<commit_message>
fixing excel count issues
</commit_message>
<xml_diff>
--- a/commonMetricsReport.xlsx
+++ b/commonMetricsReport.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Reporting Information</t>
   </si>
@@ -100,12 +100,72 @@
     <t>If not, why?</t>
   </si>
   <si>
+    <t>q1 total repsonses</t>
+  </si>
+  <si>
+    <t>q2 total repsonses</t>
+  </si>
+  <si>
+    <t>q3 total repsonses</t>
+  </si>
+  <si>
+    <t>q4 total repsonses</t>
+  </si>
+  <si>
+    <t>q5 total repsonses</t>
+  </si>
+  <si>
     <t>None</t>
   </si>
   <si>
     <t>John Doe</t>
   </si>
   <si>
+    <t>Marketing Public Health</t>
+  </si>
+  <si>
+    <t>Maintaining Safe Recreational Waters</t>
+  </si>
+  <si>
+    <t>Massachusetts Public Health Inspector Training: Housing</t>
+  </si>
+  <si>
+    <t>Monitoring for Cyanobacteria</t>
+  </si>
+  <si>
+    <t>Housing Certificate Program Final Assessment</t>
+  </si>
+  <si>
+    <t>Introduction to Outreach Methods and Strategies</t>
+  </si>
+  <si>
+    <t>Coaching Skills</t>
+  </si>
+  <si>
+    <t>Onboarding New Employees</t>
+  </si>
+  <si>
+    <t>Effective Meetings</t>
+  </si>
+  <si>
+    <t>Ten Essential Services of Public Health in Action</t>
+  </si>
+  <si>
+    <t>Grant Writing Basics</t>
+  </si>
+  <si>
+    <t>Substance Use Disorders and Models for Supporting Recovery</t>
+  </si>
+  <si>
+    <t>Community Health Assessment: Using Health Models to Explore the Determinants of Health</t>
+  </si>
+  <si>
+    <t>LPHI Emergency Preparedness Training Certificate</t>
+  </si>
+  <si>
+    <t>Numbers in Health:  Make the Meaning Clear</t>
+  </si>
+  <si>
     <t>Human Health Effects of Climate Change</t>
   </si>
   <si>
@@ -113,54 +173,6 @@
   </si>
   <si>
     <t>Introduction to Environmental Health for New Hampshire Health Officers</t>
-  </si>
-  <si>
-    <t>Marketing Public Health</t>
-  </si>
-  <si>
-    <t>Maintaining Safe Recreational Waters</t>
-  </si>
-  <si>
-    <t>Massachusetts Public Health Inspector Training: Housing</t>
-  </si>
-  <si>
-    <t>Monitoring for Cyanobacteria</t>
-  </si>
-  <si>
-    <t>Housing Certificate Program Final Assessment</t>
-  </si>
-  <si>
-    <t>Introduction to Outreach Methods and Strategies</t>
-  </si>
-  <si>
-    <t>Coaching Skills</t>
-  </si>
-  <si>
-    <t>Onboarding New Employees</t>
-  </si>
-  <si>
-    <t>Effective Meetings</t>
-  </si>
-  <si>
-    <t>Ten Essential Services of Public Health in Action</t>
-  </si>
-  <si>
-    <t>Grant Writing Basics</t>
-  </si>
-  <si>
-    <t>Substance Use Disorders and Models for Supporting Recovery</t>
-  </si>
-  <si>
-    <t>Healthcare Incident Command System: Application for Community Health Centers</t>
-  </si>
-  <si>
-    <t>Community Health Assessment: Using Health Models to Explore the Determinants of Health</t>
-  </si>
-  <si>
-    <t>LPHI Emergency Preparedness Training Certificate</t>
-  </si>
-  <si>
-    <t>Numbers in Health:  Make the Meaning Clear</t>
   </si>
 </sst>
 </file>
@@ -260,7 +272,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr/>
-  <dimension ref="A1:BJ21"/>
+  <dimension ref="A1:BO20"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -533,213 +545,243 @@
       <c r="BJ2" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="BK2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="BL2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="BM2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="BN2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="BO2" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="3" spans="3:3">
       <c r="A3" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B3" s="7">
         <v>42736</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D3" s="7">
-        <v>43091.7450717</v>
+        <v>43119.8575448</v>
       </c>
       <c r="E3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="S3" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="T3" s="0" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="U3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V3" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="W3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="Z3" s="0" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="AA3" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="AB3" s="0" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="AC3" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="AD3" s="0" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="AE3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AG3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH3" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AI3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AJ3" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AK3" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="AL3" s="0" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="AM3" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="AN3" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AO3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP3" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AQ3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="AT3" s="0" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="AU3" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="AV3" s="0" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="AW3" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="N3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="P3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="R3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="T3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="V3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="X3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="Z3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AB3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AD3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AF3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AH3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AJ3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AL3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AN3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AP3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AR3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AT3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AV3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW3" s="0" t="n">
-        <v>-1</v>
-      </c>
       <c r="AX3" s="0" t="n">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="AY3" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AZ3" s="0" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="BA3" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BB3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BC3" s="0" t="n">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="BD3" s="0" t="n">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="BE3" s="0" t="n">
-        <v>-1</v>
+        <v>41</v>
       </c>
       <c r="BF3" s="0" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BG3" s="0" t="n">
-        <v>-1</v>
+        <v>31</v>
       </c>
       <c r="BH3" s="0" t="n">
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="BI3" s="5" t="b">
         <v>true</v>
+      </c>
+      <c r="BK3" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="BL3" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="BM3" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="BN3" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="BO3" s="0" t="n">
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="4:4">
       <c r="A4" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B4" s="7">
         <v>42736</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D4" s="7">
-        <v>43091.7450717</v>
+        <v>43119.8575448</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>0</v>
@@ -751,180 +793,195 @@
         <v>0</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>0</v>
+        <v>0.23</v>
       </c>
       <c r="M4" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="N4" s="0" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="O4" s="0" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="P4" s="0" t="n">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="Q4" s="0" t="n">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="R4" s="0" t="n">
-        <v>0</v>
+        <v>0.27</v>
       </c>
       <c r="S4" s="0" t="n">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="T4" s="0" t="n">
-        <v>0</v>
+        <v>0.27</v>
       </c>
       <c r="U4" s="0" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="V4" s="0" t="n">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="W4" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Y4" s="0" t="n">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="Z4" s="0" t="n">
-        <v>0</v>
+        <v>0.32</v>
       </c>
       <c r="AA4" s="0" t="n">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="AB4" s="0" t="n">
-        <v>0</v>
+        <v>0.32</v>
       </c>
       <c r="AC4" s="0" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="AD4" s="0" t="n">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="AE4" s="0" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="AF4" s="0" t="n">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="AG4" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AH4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AI4" s="0" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="AJ4" s="0" t="n">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="AK4" s="0" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="AL4" s="0" t="n">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="AM4" s="0" t="n">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="AN4" s="0" t="n">
-        <v>0</v>
+        <v>0.27</v>
       </c>
       <c r="AO4" s="0" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="AP4" s="0" t="n">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="AQ4" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AR4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AS4" s="0" t="n">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="AT4" s="0" t="n">
-        <v>0</v>
+        <v>0.23</v>
       </c>
       <c r="AU4" s="0" t="n">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="AV4" s="0" t="n">
-        <v>0</v>
+        <v>0.27</v>
       </c>
       <c r="AW4" s="0" t="n">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="AX4" s="0" t="n">
-        <v>0</v>
+        <v>0.32</v>
       </c>
       <c r="AY4" s="0" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="AZ4" s="0" t="n">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="BA4" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="BB4" s="0" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="BC4" s="0" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="BD4" s="0" t="n">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="BE4" s="0" t="n">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="BF4" s="0" t="n">
-        <v>0</v>
+        <v>0.32</v>
       </c>
       <c r="BG4" s="0" t="n">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="BH4" s="0" t="n">
-        <v>0</v>
+        <v>0.27</v>
       </c>
       <c r="BI4" s="5" t="b">
         <v>true</v>
+      </c>
+      <c r="BK4" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="BL4" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="BM4" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="BN4" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="BO4" s="0" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="5:5">
       <c r="A5" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B5" s="7">
         <v>42736</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D5" s="7">
-        <v>43091.7450717</v>
+        <v>43119.8575448</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>0</v>
@@ -936,180 +993,195 @@
         <v>0</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="L5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M5" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O5" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="P5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Q5" s="0" t="n">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="R5" s="0" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S5" s="0" t="n">
-        <v>-1</v>
+        <v>24</v>
       </c>
       <c r="T5" s="0" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="U5" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="V5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W5" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Y5" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Z5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AA5" s="0" t="n">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="AB5" s="0" t="n">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="AC5" s="0" t="n">
-        <v>-1</v>
+        <v>25</v>
       </c>
       <c r="AD5" s="0" t="n">
-        <v>0</v>
+        <v>0.83</v>
       </c>
       <c r="AE5" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AF5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AG5" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AH5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AI5" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AJ5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AK5" s="0" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="AL5" s="0" t="n">
-        <v>0</v>
+        <v>0.27</v>
       </c>
       <c r="AM5" s="0" t="n">
-        <v>-1</v>
+        <v>22</v>
       </c>
       <c r="AN5" s="0" t="n">
-        <v>0</v>
+        <v>0.73</v>
       </c>
       <c r="AO5" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AP5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AQ5" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AR5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AS5" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AT5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AU5" s="0" t="n">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="AV5" s="0" t="n">
-        <v>0</v>
+        <v>0.23</v>
       </c>
       <c r="AW5" s="0" t="n">
-        <v>-1</v>
+        <v>23</v>
       </c>
       <c r="AX5" s="0" t="n">
-        <v>0</v>
+        <v>0.77</v>
       </c>
       <c r="AY5" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AZ5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BA5" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BB5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BC5" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BD5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BE5" s="0" t="n">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="BF5" s="0" t="n">
-        <v>0</v>
+        <v>0.64</v>
       </c>
       <c r="BG5" s="0" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="BH5" s="0" t="n">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="BI5" s="5" t="b">
         <v>true</v>
+      </c>
+      <c r="BK5" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="BL5" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="BM5" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="BN5" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="BO5" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="6:6">
       <c r="A6" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B6" s="7">
         <v>42736</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D6" s="7">
-        <v>43091.7450717</v>
+        <v>43119.8575448</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>0</v>
@@ -1121,180 +1193,195 @@
         <v>0</v>
       </c>
       <c r="K6" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="L6" s="0" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="M6" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="N6" s="0" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="O6" s="0" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="P6" s="0" t="n">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="Q6" s="0" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="R6" s="0" t="n">
-        <v>0</v>
+        <v>0.21</v>
       </c>
       <c r="S6" s="0" t="n">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="T6" s="0" t="n">
-        <v>0</v>
+        <v>0.53</v>
       </c>
       <c r="U6" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="V6" s="0" t="n">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="W6" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Y6" s="0" t="n">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="Z6" s="0" t="n">
-        <v>0</v>
+        <v>0.47</v>
       </c>
       <c r="AA6" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AB6" s="0" t="n">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="AC6" s="0" t="n">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="AD6" s="0" t="n">
-        <v>0</v>
+        <v>0.32</v>
       </c>
       <c r="AE6" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AF6" s="0" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AG6" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AH6" s="0" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AI6" s="0" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="AJ6" s="0" t="n">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="AK6" s="0" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="AL6" s="0" t="n">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="AM6" s="0" t="n">
-        <v>-1</v>
+        <v>11</v>
       </c>
       <c r="AN6" s="0" t="n">
-        <v>0</v>
+        <v>0.58</v>
       </c>
       <c r="AO6" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AP6" s="0" t="n">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="AQ6" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AR6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AS6" s="0" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="AT6" s="0" t="n">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="AU6" s="0" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="AV6" s="0" t="n">
-        <v>0</v>
+        <v>0.21</v>
       </c>
       <c r="AW6" s="0" t="n">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="AX6" s="0" t="n">
-        <v>0</v>
+        <v>0.53</v>
       </c>
       <c r="AY6" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AZ6" s="0" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="BA6" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BB6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BC6" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="BD6" s="0" t="n">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="BE6" s="0" t="n">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="BF6" s="0" t="n">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="BG6" s="0" t="n">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="BH6" s="0" t="n">
-        <v>0</v>
+        <v>0.47</v>
       </c>
       <c r="BI6" s="5" t="b">
         <v>true</v>
+      </c>
+      <c r="BK6" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="BL6" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="BM6" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="BN6" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="BO6" s="0" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="7:7">
       <c r="A7" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B7" s="7">
         <v>42736</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D7" s="7">
-        <v>43091.7450717</v>
+        <v>43119.8575448</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>0</v>
@@ -1306,180 +1393,195 @@
         <v>0</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="L7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M7" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O7" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="P7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Q7" s="0" t="n">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="R7" s="0" t="n">
-        <v>0</v>
+        <v>0.64</v>
       </c>
       <c r="S7" s="0" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="T7" s="0" t="n">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="U7" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="V7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W7" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Y7" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Z7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AA7" s="0" t="n">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="AB7" s="0" t="n">
-        <v>0</v>
+        <v>0.64</v>
       </c>
       <c r="AC7" s="0" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="AD7" s="0" t="n">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="AE7" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AF7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AG7" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AH7" s="0" t="n">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="AI7" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AJ7" s="0" t="n">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="AK7" s="0" t="n">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="AL7" s="0" t="n">
-        <v>0</v>
+        <v>0.55</v>
       </c>
       <c r="AM7" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AN7" s="0" t="n">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="AO7" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AP7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AQ7" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AR7" s="0" t="n">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="AS7" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AT7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AU7" s="0" t="n">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="AV7" s="0" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="AW7" s="0" t="n">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="AX7" s="0" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="AY7" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AZ7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BA7" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BB7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BC7" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="BD7" s="0" t="n">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="BE7" s="0" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="BF7" s="0" t="n">
-        <v>0</v>
+        <v>0.73</v>
       </c>
       <c r="BG7" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="BH7" s="0" t="n">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="BI7" s="5" t="b">
         <v>true</v>
+      </c>
+      <c r="BK7" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="BL7" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="BM7" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="BN7" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="BO7" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="8:8">
       <c r="A8" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B8" s="7">
         <v>42736</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D8" s="7">
-        <v>43091.7450717</v>
+        <v>43119.8575448</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>0</v>
@@ -1491,550 +1593,595 @@
         <v>0</v>
       </c>
       <c r="K8" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="L8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M8" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O8" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="P8" s="0" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="Q8" s="0" t="n">
-        <v>-1</v>
+        <v>24</v>
       </c>
       <c r="R8" s="0" t="n">
-        <v>0</v>
+        <v>0.57</v>
       </c>
       <c r="S8" s="0" t="n">
-        <v>-1</v>
+        <v>16</v>
       </c>
       <c r="T8" s="0" t="n">
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="U8" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="V8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W8" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Y8" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Z8" s="0" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="AA8" s="0" t="n">
-        <v>-1</v>
+        <v>24</v>
       </c>
       <c r="AB8" s="0" t="n">
-        <v>0</v>
+        <v>0.57</v>
       </c>
       <c r="AC8" s="0" t="n">
-        <v>-1</v>
+        <v>17</v>
       </c>
       <c r="AD8" s="0" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="AE8" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AF8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AG8" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AH8" s="0" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="AI8" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AJ8" s="0" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AK8" s="0" t="n">
-        <v>-1</v>
+        <v>21</v>
       </c>
       <c r="AL8" s="0" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AM8" s="0" t="n">
-        <v>-1</v>
+        <v>18</v>
       </c>
       <c r="AN8" s="0" t="n">
-        <v>0</v>
+        <v>0.43</v>
       </c>
       <c r="AO8" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AP8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AQ8" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AR8" s="0" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="AS8" s="0" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="AT8" s="0" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AU8" s="0" t="n">
-        <v>-1</v>
+        <v>21</v>
       </c>
       <c r="AV8" s="0" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AW8" s="0" t="n">
-        <v>-1</v>
+        <v>16</v>
       </c>
       <c r="AX8" s="0" t="n">
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="AY8" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AZ8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BA8" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BB8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BC8" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="BD8" s="0" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="BE8" s="0" t="n">
-        <v>-1</v>
+        <v>21</v>
       </c>
       <c r="BF8" s="0" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BG8" s="0" t="n">
-        <v>-1</v>
+        <v>19</v>
       </c>
       <c r="BH8" s="0" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="BI8" s="5" t="b">
         <v>true</v>
+      </c>
+      <c r="BK8" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="BL8" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="BM8" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="BN8" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="BO8" s="0" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="9:9">
       <c r="A9" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B9" s="7">
         <v>42736</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="7">
+        <v>43119.8575448</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="S9" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="T9" s="0" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="U9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="V9" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="W9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z9" s="0" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="AA9" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="AB9" s="0" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="AC9" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="AD9" s="0" t="n">
+        <v>0.56</v>
+      </c>
+      <c r="AE9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF9" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AG9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ9" s="0" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="AK9" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="AL9" s="0" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="AM9" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="AN9" s="0" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="AO9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP9" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AQ9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AT9" s="0" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="AU9" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="AV9" s="0" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="AW9" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="AX9" s="0" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="AY9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AZ9" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="BA9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BD9" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BE9" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="D9" s="7">
-        <v>43091.7450717</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="L9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="N9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="P9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="R9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="T9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="V9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="X9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="Z9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AB9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AD9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AF9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AH9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AJ9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AL9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AN9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AP9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AR9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AT9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AV9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AX9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AZ9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="BB9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="BD9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE9" s="0" t="n">
-        <v>-1</v>
-      </c>
       <c r="BF9" s="0" t="n">
-        <v>0</v>
+        <v>0.42</v>
       </c>
       <c r="BG9" s="0" t="n">
-        <v>-1</v>
+        <v>39</v>
       </c>
       <c r="BH9" s="0" t="n">
-        <v>0</v>
+        <v>0.54</v>
       </c>
       <c r="BI9" s="5" t="b">
         <v>true</v>
+      </c>
+      <c r="BK9" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="BL9" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="BM9" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="BN9" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="BO9" s="0" t="n">
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="10:10">
       <c r="A10" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B10" s="7">
         <v>42736</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D10" s="7">
-        <v>43091.7450717</v>
+        <v>43119.8575448</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="S10" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="T10" s="0" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="U10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z10" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="AA10" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB10" s="0" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="AC10" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="AD10" s="0" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="AE10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ10" s="0" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK10" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="AL10" s="0" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="AM10" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="L10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="N10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="P10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="R10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S10" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="T10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U10" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="V10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W10" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="X10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="Z10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AB10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AD10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE10" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AF10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG10" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AH10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI10" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AJ10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK10" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AL10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM10" s="0" t="n">
-        <v>-1</v>
-      </c>
       <c r="AN10" s="0" t="n">
-        <v>0</v>
+        <v>0.54</v>
       </c>
       <c r="AO10" s="0" t="n">
         <v>-1</v>
       </c>
       <c r="AP10" s="0" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AQ10" s="0" t="n">
         <v>-1</v>
       </c>
       <c r="AR10" s="0" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AS10" s="0" t="n">
         <v>-1</v>
       </c>
       <c r="AT10" s="0" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AU10" s="0" t="n">
         <v>-1</v>
       </c>
       <c r="AV10" s="0" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AW10" s="0" t="n">
         <v>-1</v>
       </c>
       <c r="AX10" s="0" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AY10" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AZ10" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BA10" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BB10" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BC10" s="0" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="BD10" s="0" t="n">
-        <v>0</v>
+        <v>0.07</v>
       </c>
       <c r="BE10" s="0" t="n">
-        <v>-1</v>
+        <v>18</v>
       </c>
       <c r="BF10" s="0" t="n">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="BG10" s="0" t="n">
-        <v>-1</v>
+        <v>32</v>
       </c>
       <c r="BH10" s="0" t="n">
-        <v>0</v>
+        <v>0.59</v>
       </c>
       <c r="BI10" s="5" t="b">
         <v>true</v>
+      </c>
+      <c r="BK10" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="BL10" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="BM10" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="BN10" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="BO10" s="0" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="11:11">
       <c r="A11" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B11" s="7">
         <v>42736</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D11" s="7">
-        <v>43091.7450717</v>
+        <v>43119.8575448</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>0</v>
@@ -2046,180 +2193,195 @@
         <v>0</v>
       </c>
       <c r="K11" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="L11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M11" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="N11" s="0" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="O11" s="0" t="n">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="P11" s="0" t="n">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="Q11" s="0" t="n">
-        <v>-1</v>
+        <v>19</v>
       </c>
       <c r="R11" s="0" t="n">
-        <v>0</v>
+        <v>0.42</v>
       </c>
       <c r="S11" s="0" t="n">
-        <v>-1</v>
+        <v>20</v>
       </c>
       <c r="T11" s="0" t="n">
-        <v>0</v>
+        <v>0.44</v>
       </c>
       <c r="U11" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="V11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W11" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X11" s="0" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="Y11" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="Z11" s="0" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="AA11" s="0" t="n">
-        <v>-1</v>
+        <v>23</v>
       </c>
       <c r="AB11" s="0" t="n">
-        <v>0</v>
+        <v>0.51</v>
       </c>
       <c r="AC11" s="0" t="n">
-        <v>-1</v>
+        <v>19</v>
       </c>
       <c r="AD11" s="0" t="n">
-        <v>0</v>
+        <v>0.42</v>
       </c>
       <c r="AE11" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AF11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AG11" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AH11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AI11" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AJ11" s="0" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="AK11" s="0" t="n">
-        <v>-1</v>
+        <v>17</v>
       </c>
       <c r="AL11" s="0" t="n">
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="AM11" s="0" t="n">
-        <v>-1</v>
+        <v>27</v>
       </c>
       <c r="AN11" s="0" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="AO11" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AP11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AQ11" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AR11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AS11" s="0" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="AT11" s="0" t="n">
-        <v>0</v>
+        <v>0.07</v>
       </c>
       <c r="AU11" s="0" t="n">
-        <v>-1</v>
+        <v>19</v>
       </c>
       <c r="AV11" s="0" t="n">
-        <v>0</v>
+        <v>0.42</v>
       </c>
       <c r="AW11" s="0" t="n">
-        <v>-1</v>
+        <v>23</v>
       </c>
       <c r="AX11" s="0" t="n">
-        <v>0</v>
+        <v>0.51</v>
       </c>
       <c r="AY11" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AZ11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BA11" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BB11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BC11" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="BD11" s="0" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="BE11" s="0" t="n">
-        <v>-1</v>
+        <v>20</v>
       </c>
       <c r="BF11" s="0" t="n">
-        <v>0</v>
+        <v>0.44</v>
       </c>
       <c r="BG11" s="0" t="n">
-        <v>-1</v>
+        <v>23</v>
       </c>
       <c r="BH11" s="0" t="n">
-        <v>0</v>
+        <v>0.51</v>
       </c>
       <c r="BI11" s="5" t="b">
         <v>true</v>
+      </c>
+      <c r="BK11" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="BL11" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="BM11" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="BN11" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="BO11" s="0" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="12:12">
       <c r="A12" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B12" s="7">
         <v>42736</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D12" s="7">
-        <v>43091.7450717</v>
+        <v>43119.8575448</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>0</v>
@@ -2231,180 +2393,195 @@
         <v>0</v>
       </c>
       <c r="K12" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="L12" s="0" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="M12" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N12" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O12" s="0" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="P12" s="0" t="n">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="Q12" s="0" t="n">
-        <v>-1</v>
+        <v>24</v>
       </c>
       <c r="R12" s="0" t="n">
-        <v>0</v>
+        <v>0.52</v>
       </c>
       <c r="S12" s="0" t="n">
-        <v>-1</v>
+        <v>16</v>
       </c>
       <c r="T12" s="0" t="n">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="U12" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="V12" s="0" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="W12" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X12" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Y12" s="0" t="n">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="Z12" s="0" t="n">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="AA12" s="0" t="n">
-        <v>-1</v>
+        <v>24</v>
       </c>
       <c r="AB12" s="0" t="n">
-        <v>0</v>
+        <v>0.52</v>
       </c>
       <c r="AC12" s="0" t="n">
-        <v>-1</v>
+        <v>14</v>
       </c>
       <c r="AD12" s="0" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="AE12" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AF12" s="0" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="AG12" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AH12" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AI12" s="0" t="n">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="AJ12" s="0" t="n">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="AK12" s="0" t="n">
-        <v>-1</v>
+        <v>21</v>
       </c>
       <c r="AL12" s="0" t="n">
-        <v>0</v>
+        <v>0.46</v>
       </c>
       <c r="AM12" s="0" t="n">
-        <v>-1</v>
+        <v>16</v>
       </c>
       <c r="AN12" s="0" t="n">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="AO12" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AP12" s="0" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="AQ12" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AR12" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AS12" s="0" t="n">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="AT12" s="0" t="n">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="AU12" s="0" t="n">
-        <v>-1</v>
+        <v>21</v>
       </c>
       <c r="AV12" s="0" t="n">
-        <v>0</v>
+        <v>0.46</v>
       </c>
       <c r="AW12" s="0" t="n">
-        <v>-1</v>
+        <v>17</v>
       </c>
       <c r="AX12" s="0" t="n">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="AY12" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AZ12" s="0" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="BA12" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BB12" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BC12" s="0" t="n">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="BD12" s="0" t="n">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="BE12" s="0" t="n">
-        <v>-1</v>
+        <v>21</v>
       </c>
       <c r="BF12" s="0" t="n">
-        <v>0</v>
+        <v>0.46</v>
       </c>
       <c r="BG12" s="0" t="n">
-        <v>-1</v>
+        <v>18</v>
       </c>
       <c r="BH12" s="0" t="n">
-        <v>0</v>
+        <v>0.39</v>
       </c>
       <c r="BI12" s="5" t="b">
         <v>true</v>
+      </c>
+      <c r="BK12" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="BL12" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="BM12" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="BN12" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="BO12" s="0" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="13:13">
       <c r="A13" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B13" s="7">
         <v>42736</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D13" s="7">
-        <v>43091.7450717</v>
+        <v>43119.8575448</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>0</v>
@@ -2416,180 +2593,195 @@
         <v>0</v>
       </c>
       <c r="K13" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="L13" s="0" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="M13" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="N13" s="0" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="O13" s="0" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="P13" s="0" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="Q13" s="0" t="n">
-        <v>-1</v>
+        <v>32</v>
       </c>
       <c r="R13" s="0" t="n">
-        <v>0</v>
+        <v>0.49</v>
       </c>
       <c r="S13" s="0" t="n">
-        <v>-1</v>
+        <v>25</v>
       </c>
       <c r="T13" s="0" t="n">
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="U13" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="V13" s="0" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="W13" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="X13" s="0" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="Y13" s="0" t="n">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="Z13" s="0" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="AA13" s="0" t="n">
-        <v>-1</v>
+        <v>34</v>
       </c>
       <c r="AB13" s="0" t="n">
-        <v>0</v>
+        <v>0.52</v>
       </c>
       <c r="AC13" s="0" t="n">
-        <v>-1</v>
+        <v>18</v>
       </c>
       <c r="AD13" s="0" t="n">
-        <v>0</v>
+        <v>0.28</v>
       </c>
       <c r="AE13" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AF13" s="0" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="AG13" s="0" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="AH13" s="0" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AI13" s="0" t="n">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="AJ13" s="0" t="n">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="AK13" s="0" t="n">
-        <v>-1</v>
+        <v>31</v>
       </c>
       <c r="AL13" s="0" t="n">
-        <v>0</v>
+        <v>0.48</v>
       </c>
       <c r="AM13" s="0" t="n">
-        <v>-1</v>
+        <v>22</v>
       </c>
       <c r="AN13" s="0" t="n">
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="AO13" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AP13" s="0" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="AQ13" s="0" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="AR13" s="0" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="AS13" s="0" t="n">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="AT13" s="0" t="n">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="AU13" s="0" t="n">
-        <v>-1</v>
+        <v>28</v>
       </c>
       <c r="AV13" s="0" t="n">
-        <v>0</v>
+        <v>0.43</v>
       </c>
       <c r="AW13" s="0" t="n">
-        <v>-1</v>
+        <v>24</v>
       </c>
       <c r="AX13" s="0" t="n">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="AY13" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AZ13" s="0" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="BA13" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="BB13" s="0" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="BC13" s="0" t="n">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="BD13" s="0" t="n">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="BE13" s="0" t="n">
-        <v>-1</v>
+        <v>31</v>
       </c>
       <c r="BF13" s="0" t="n">
-        <v>0</v>
+        <v>0.48</v>
       </c>
       <c r="BG13" s="0" t="n">
-        <v>-1</v>
+        <v>24</v>
       </c>
       <c r="BH13" s="0" t="n">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="BI13" s="5" t="b">
         <v>true</v>
+      </c>
+      <c r="BK13" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="BL13" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="BM13" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="BN13" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="BO13" s="0" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="14:14">
       <c r="A14" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B14" s="7">
         <v>42736</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D14" s="7">
-        <v>43091.7450717</v>
+        <v>43119.8575448</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>0</v>
@@ -2601,180 +2793,195 @@
         <v>0</v>
       </c>
       <c r="K14" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="L14" s="0" t="n">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="M14" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O14" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="P14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Q14" s="0" t="n">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="R14" s="0" t="n">
-        <v>0</v>
+        <v>0.26</v>
       </c>
       <c r="S14" s="0" t="n">
-        <v>-1</v>
+        <v>12</v>
       </c>
       <c r="T14" s="0" t="n">
-        <v>0</v>
+        <v>0.63</v>
       </c>
       <c r="U14" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="V14" s="0" t="n">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="W14" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Y14" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Z14" s="0" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AA14" s="0" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="AB14" s="0" t="n">
-        <v>0</v>
+        <v>0.21</v>
       </c>
       <c r="AC14" s="0" t="n">
-        <v>-1</v>
+        <v>12</v>
       </c>
       <c r="AD14" s="0" t="n">
-        <v>0</v>
+        <v>0.63</v>
       </c>
       <c r="AE14" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AF14" s="0" t="n">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="AG14" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AH14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AI14" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AJ14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AK14" s="0" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="AL14" s="0" t="n">
-        <v>0</v>
+        <v>0.21</v>
       </c>
       <c r="AM14" s="0" t="n">
-        <v>-1</v>
+        <v>13</v>
       </c>
       <c r="AN14" s="0" t="n">
-        <v>0</v>
+        <v>0.68</v>
       </c>
       <c r="AO14" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AP14" s="0" t="n">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="AQ14" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AR14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AS14" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AT14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AU14" s="0" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="AV14" s="0" t="n">
-        <v>0</v>
+        <v>0.21</v>
       </c>
       <c r="AW14" s="0" t="n">
-        <v>-1</v>
+        <v>13</v>
       </c>
       <c r="AX14" s="0" t="n">
-        <v>0</v>
+        <v>0.68</v>
       </c>
       <c r="AY14" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AZ14" s="0" t="n">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="BA14" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BB14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BC14" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BD14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BE14" s="0" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="BF14" s="0" t="n">
-        <v>0</v>
+        <v>0.21</v>
       </c>
       <c r="BG14" s="0" t="n">
-        <v>-1</v>
+        <v>13</v>
       </c>
       <c r="BH14" s="0" t="n">
-        <v>0</v>
+        <v>0.68</v>
       </c>
       <c r="BI14" s="5" t="b">
         <v>true</v>
+      </c>
+      <c r="BK14" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="BL14" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="BM14" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="BN14" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="BO14" s="0" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="15:15">
       <c r="A15" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B15" s="7">
         <v>42736</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D15" s="7">
-        <v>43091.7450717</v>
+        <v>43119.8575448</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>0</v>
@@ -2786,180 +2993,195 @@
         <v>0</v>
       </c>
       <c r="K15" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="L15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M15" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O15" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="P15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Q15" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="R15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="S15" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="T15" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U15" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="V15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W15" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Y15" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Z15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AA15" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AC15" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AD15" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE15" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AF15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AG15" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AH15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AI15" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AJ15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AK15" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AL15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AM15" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AN15" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO15" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AP15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AQ15" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AR15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AS15" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AT15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AU15" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AV15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AW15" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AX15" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY15" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AZ15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BA15" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BB15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BC15" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BD15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BE15" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BF15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BG15" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="BH15" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI15" s="5" t="b">
         <v>true</v>
+      </c>
+      <c r="BK15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BL15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BM15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO15" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="16:16">
       <c r="A16" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B16" s="7">
         <v>42736</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D16" s="7">
-        <v>43091.7450717</v>
+        <v>43119.8575448</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>0</v>
@@ -2971,180 +3193,195 @@
         <v>0</v>
       </c>
       <c r="K16" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="L16" s="0" t="n">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="M16" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O16" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="P16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Q16" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="R16" s="0" t="n">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="S16" s="0" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="T16" s="0" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="U16" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="V16" s="0" t="n">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="W16" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Y16" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Z16" s="0" t="n">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="AA16" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AB16" s="0" t="n">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="AC16" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AD16" s="0" t="n">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="AE16" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AF16" s="0" t="n">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="AG16" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AH16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AI16" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AJ16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AK16" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AL16" s="0" t="n">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="AM16" s="0" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="AN16" s="0" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AO16" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AP16" s="0" t="n">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="AQ16" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AR16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AS16" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AT16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AU16" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AV16" s="0" t="n">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="AW16" s="0" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="AX16" s="0" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AY16" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AZ16" s="0" t="n">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="BA16" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BB16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BC16" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BD16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BE16" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="BF16" s="0" t="n">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="BG16" s="0" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="BH16" s="0" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BI16" s="5" t="b">
         <v>true</v>
+      </c>
+      <c r="BK16" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="BL16" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="BM16" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="BN16" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="BO16" s="0" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="17:17">
       <c r="A17" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B17" s="7">
         <v>42736</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D17" s="7">
-        <v>43091.7450717</v>
+        <v>43119.8575448</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H17" s="0" t="n">
         <v>0</v>
@@ -3156,180 +3393,195 @@
         <v>0</v>
       </c>
       <c r="K17" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="L17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M17" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O17" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="P17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Q17" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="R17" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S17" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="U17" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="V17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W17" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Y17" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Z17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AA17" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AB17" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC17" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AD17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AE17" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AF17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AG17" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AH17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AI17" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AJ17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AK17" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AL17" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM17" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AN17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AO17" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AP17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AQ17" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AR17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AS17" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AT17" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU17" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AV17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AW17" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AX17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AY17" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AZ17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BA17" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BB17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BC17" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BD17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BE17" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="BF17" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG17" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BH17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BI17" s="5" t="b">
         <v>true</v>
+      </c>
+      <c r="BK17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BL17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BM17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO17" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="18:18">
       <c r="A18" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B18" s="7">
         <v>42736</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D18" s="7">
-        <v>43091.7450717</v>
+        <v>43119.8575448</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H18" s="0" t="n">
         <v>0</v>
@@ -3341,180 +3593,195 @@
         <v>0</v>
       </c>
       <c r="K18" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="L18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M18" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O18" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="P18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Q18" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="R18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="S18" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="T18" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U18" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="V18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W18" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Y18" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Z18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AA18" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AB18" s="0" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AC18" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AD18" s="0" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AE18" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AF18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AG18" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AH18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AI18" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AJ18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AK18" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AL18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AM18" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AN18" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO18" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AP18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AQ18" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AR18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AS18" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AT18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AU18" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AV18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AW18" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AX18" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY18" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AZ18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BA18" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BB18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BC18" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BD18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BE18" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BF18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BG18" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="BH18" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI18" s="5" t="b">
         <v>true</v>
+      </c>
+      <c r="BK18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="BL18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="BM18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="BN18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="BO18" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="19:19">
       <c r="A19" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B19" s="7">
         <v>42736</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D19" s="7">
-        <v>43091.7450717</v>
+        <v>43119.8575448</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H19" s="0" t="n">
         <v>0</v>
@@ -3526,180 +3793,195 @@
         <v>0</v>
       </c>
       <c r="K19" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="L19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M19" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O19" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="P19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Q19" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="R19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="S19" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="T19" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U19" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="V19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W19" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Y19" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Z19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AA19" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AC19" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AD19" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE19" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AF19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AG19" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AH19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AI19" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AJ19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AK19" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AL19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AM19" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AN19" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO19" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AP19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AQ19" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AR19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AS19" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AT19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AU19" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AV19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AW19" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AX19" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY19" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AZ19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BA19" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BB19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BC19" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BD19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BE19" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BF19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BG19" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="BH19" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI19" s="5" t="b">
         <v>true</v>
+      </c>
+      <c r="BK19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BL19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BM19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO19" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="20:20">
       <c r="A20" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B20" s="7">
         <v>42736</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D20" s="7">
-        <v>43091.7450717</v>
+        <v>43119.8575448</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H20" s="0" t="n">
         <v>0</v>
@@ -3711,151 +3993,151 @@
         <v>0</v>
       </c>
       <c r="K20" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="L20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M20" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O20" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="P20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Q20" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="R20" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S20" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="U20" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="V20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W20" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Y20" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Z20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AA20" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AC20" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AD20" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE20" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AF20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AG20" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AH20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AI20" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AJ20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AK20" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AL20" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM20" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AN20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AO20" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AP20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AQ20" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AR20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AS20" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AT20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AU20" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AV20" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW20" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AX20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AY20" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AZ20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BA20" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BB20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BC20" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BD20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="BE20" s="0" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="BF20" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG20" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BH20" s="0" t="n">
         <v>0</v>
@@ -3863,190 +4145,20 @@
       <c r="BI20" s="5" t="b">
         <v>true</v>
       </c>
-    </row>
-    <row r="21" spans="21:21">
-      <c r="A21" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="7">
-        <v>42736</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="7">
-        <v>43091.7450717</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="L21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="N21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="P21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="R21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="T21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="V21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="X21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="Z21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AB21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AD21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AF21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AH21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AJ21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AL21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AN21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AP21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AR21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AT21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AV21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AX21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AZ21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="BB21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="BD21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="BF21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="BH21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BI21" s="5" t="b">
-        <v>true</v>
+      <c r="BK20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BL20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BM20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO20" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished common metrics bug issue - common metrics table - ehb table 90 percent
</commit_message>
<xml_diff>
--- a/commonMetricsReport.xlsx
+++ b/commonMetricsReport.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Reporting Information</t>
   </si>
@@ -22,16 +22,16 @@
     <t>Q1: Subject Matter Understanding Improved</t>
   </si>
   <si>
-    <t>Q2: Subject Matter Understanding Improved</t>
-  </si>
-  <si>
-    <t>Q3: Subject Matter Understanding Improved</t>
-  </si>
-  <si>
-    <t>Q4: Subject Matter Understanding Improved</t>
-  </si>
-  <si>
-    <t>Q5: Subject Matter Understanding Improved</t>
+    <t>Q2: Identified Actions to Apply Information</t>
+  </si>
+  <si>
+    <t>Q3: Information Was Presented Clearly</t>
+  </si>
+  <si>
+    <t>Q4: Overall Satisfaction</t>
+  </si>
+  <si>
+    <t>Q5: Learning Objecties Were Met</t>
   </si>
   <si>
     <t>Common Metrics Data Collected?</t>
@@ -100,27 +100,15 @@
     <t>If not, why?</t>
   </si>
   <si>
-    <t>q1 total repsonses</t>
-  </si>
-  <si>
-    <t>q2 total repsonses</t>
-  </si>
-  <si>
-    <t>q3 total repsonses</t>
-  </si>
-  <si>
-    <t>q4 total repsonses</t>
-  </si>
-  <si>
-    <t>q5 total repsonses</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
     <t>John Doe</t>
   </si>
   <si>
+    <t>Onboarding New Employees</t>
+  </si>
+  <si>
     <t>Marketing Public Health</t>
   </si>
   <si>
@@ -140,9 +128,6 @@
   </si>
   <si>
     <t>Coaching Skills</t>
-  </si>
-  <si>
-    <t>Onboarding New Employees</t>
   </si>
   <si>
     <t>Effective Meetings</t>
@@ -272,7 +257,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr/>
-  <dimension ref="A1:BO20"/>
+  <dimension ref="A1:BJ20"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -545,58 +530,43 @@
       <c r="BJ2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="BK2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="BL2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="BM2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="BN2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="BO2" s="3" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="3" spans="3:3">
       <c r="A3" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B3" s="7">
         <v>42736</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D3" s="7">
-        <v>43119.8575448</v>
+        <v>43126.7719773</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="M3" s="0" t="n">
         <v>0</v>
@@ -605,28 +575,28 @@
         <v>0</v>
       </c>
       <c r="O3" s="0" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="P3" s="0" t="n">
-        <v>0.13</v>
+        <v>9</v>
       </c>
       <c r="Q3" s="0" t="n">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="R3" s="0" t="n">
-        <v>0.48</v>
+        <v>43</v>
       </c>
       <c r="S3" s="0" t="n">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="T3" s="0" t="n">
-        <v>0.38</v>
+        <v>48</v>
       </c>
       <c r="U3" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V3" s="0" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="W3" s="0" t="n">
         <v>0</v>
@@ -635,398 +605,368 @@
         <v>0</v>
       </c>
       <c r="Y3" s="0" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="Z3" s="0" t="n">
-        <v>0.15</v>
+        <v>7.000000000000001</v>
       </c>
       <c r="AA3" s="0" t="n">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="AB3" s="0" t="n">
-        <v>0.55</v>
+        <v>46</v>
       </c>
       <c r="AC3" s="0" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AD3" s="0" t="n">
-        <v>0.29</v>
+        <v>46</v>
       </c>
       <c r="AE3" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF3" s="0" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="AG3" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH3" s="0" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="AI3" s="0" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="AJ3" s="0" t="n">
-        <v>0.1</v>
+        <v>6</v>
       </c>
       <c r="AK3" s="0" t="n">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="AL3" s="0" t="n">
-        <v>0.46</v>
+        <v>41</v>
       </c>
       <c r="AM3" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="AN3" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="AO3" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AP3" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AQ3" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AR3" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AS3" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AT3" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AU3" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AV3" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AW3" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AX3" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AY3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="BD3" s="0" t="n">
+        <v>7.000000000000001</v>
+      </c>
+      <c r="BE3" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="BF3" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="AN3" s="0" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="AO3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="AP3" s="0" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="AQ3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="AT3" s="0" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="AU3" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="AV3" s="0" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="AW3" s="0" t="n">
-        <v>29</v>
-      </c>
-      <c r="AX3" s="0" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="AY3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ3" s="0" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="BA3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC3" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="BD3" s="0" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="BE3" s="0" t="n">
-        <v>41</v>
-      </c>
-      <c r="BF3" s="0" t="n">
-        <v>0.5</v>
-      </c>
       <c r="BG3" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="BH3" s="0" t="n">
-        <v>0.38</v>
+        <v>59</v>
       </c>
       <c r="BI3" s="5" t="b">
         <v>true</v>
-      </c>
-      <c r="BK3" s="0" t="n">
-        <v>82</v>
-      </c>
-      <c r="BL3" s="0" t="n">
-        <v>82</v>
-      </c>
-      <c r="BM3" s="0" t="n">
-        <v>82</v>
-      </c>
-      <c r="BN3" s="0" t="n">
-        <v>82</v>
-      </c>
-      <c r="BO3" s="0" t="n">
-        <v>82</v>
       </c>
     </row>
     <row r="4" spans="4:4">
       <c r="A4" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B4" s="7">
         <v>42736</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="7">
+        <v>43126.7719773</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>121</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="U4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="W4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="Z4" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="AA4" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="AB4" s="0" t="n">
+        <v>55.00000000000001</v>
+      </c>
+      <c r="AC4" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="AD4" s="0" t="n">
+        <v>28.999999999999996</v>
+      </c>
+      <c r="AE4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI4" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AJ4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="AK4" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="AL4" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="AM4" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="AN4" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="AO4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AQ4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="AT4" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="AU4" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="AV4" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="AW4" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="AX4" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="D4" s="7">
-        <v>43119.8575448</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="M4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N4" s="0" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="O4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="P4" s="0" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="Q4" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="R4" s="0" t="n">
-        <v>0.27</v>
-      </c>
-      <c r="S4" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="T4" s="0" t="n">
-        <v>0.27</v>
-      </c>
-      <c r="U4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="V4" s="0" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="W4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="Z4" s="0" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="AA4" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="AB4" s="0" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="AC4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD4" s="0" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="AE4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="AF4" s="0" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="AG4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="AJ4" s="0" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="AK4" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="AL4" s="0" t="n">
-        <v>0.36</v>
-      </c>
-      <c r="AM4" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="AN4" s="0" t="n">
-        <v>0.27</v>
-      </c>
-      <c r="AO4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="AP4" s="0" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="AQ4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS4" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="AT4" s="0" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="AU4" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="AV4" s="0" t="n">
-        <v>0.27</v>
-      </c>
-      <c r="AW4" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="AX4" s="0" t="n">
-        <v>0.32</v>
-      </c>
       <c r="AY4" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AZ4" s="0" t="n">
-        <v>0.18</v>
+        <v>1</v>
       </c>
       <c r="BA4" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB4" s="0" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="BC4" s="0" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="BD4" s="0" t="n">
-        <v>0.18</v>
+        <v>11</v>
       </c>
       <c r="BE4" s="0" t="n">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="BF4" s="0" t="n">
-        <v>0.32</v>
+        <v>50</v>
       </c>
       <c r="BG4" s="0" t="n">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="BH4" s="0" t="n">
-        <v>0.27</v>
+        <v>38</v>
       </c>
       <c r="BI4" s="5" t="b">
         <v>true</v>
-      </c>
-      <c r="BK4" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="BL4" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="BM4" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="BN4" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="BO4" s="0" t="n">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="5:5">
       <c r="A5" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B5" s="7">
         <v>42736</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D5" s="7">
-        <v>43119.8575448</v>
+        <v>43126.7719773</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L5" s="0" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="M5" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O5" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P5" s="0" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="Q5" s="0" t="n">
         <v>6</v>
       </c>
       <c r="R5" s="0" t="n">
-        <v>0.2</v>
+        <v>27</v>
       </c>
       <c r="S5" s="0" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="T5" s="0" t="n">
-        <v>0.8</v>
+        <v>27</v>
       </c>
       <c r="U5" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V5" s="0" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="W5" s="0" t="n">
         <v>0</v>
@@ -1035,28 +975,28 @@
         <v>0</v>
       </c>
       <c r="Y5" s="0" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Z5" s="0" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="AA5" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AB5" s="0" t="n">
-        <v>0.17</v>
+        <v>32</v>
       </c>
       <c r="AC5" s="0" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="AD5" s="0" t="n">
-        <v>0.83</v>
+        <v>18</v>
       </c>
       <c r="AE5" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AF5" s="0" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AG5" s="0" t="n">
         <v>0</v>
@@ -1065,28 +1005,28 @@
         <v>0</v>
       </c>
       <c r="AI5" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AJ5" s="0" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AK5" s="0" t="n">
         <v>8</v>
       </c>
       <c r="AL5" s="0" t="n">
-        <v>0.27</v>
+        <v>36</v>
       </c>
       <c r="AM5" s="0" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="AN5" s="0" t="n">
-        <v>0.73</v>
+        <v>27</v>
       </c>
       <c r="AO5" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AP5" s="0" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AQ5" s="0" t="n">
         <v>0</v>
@@ -1095,138 +1035,123 @@
         <v>0</v>
       </c>
       <c r="AS5" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AT5" s="0" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="AU5" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AV5" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="AW5" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="AV5" s="0" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="AW5" s="0" t="n">
-        <v>23</v>
-      </c>
       <c r="AX5" s="0" t="n">
-        <v>0.77</v>
+        <v>32</v>
       </c>
       <c r="AY5" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AZ5" s="0" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="BA5" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB5" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BC5" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BD5" s="0" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="BE5" s="0" t="n">
         <v>7</v>
       </c>
       <c r="BF5" s="0" t="n">
-        <v>0.64</v>
+        <v>32</v>
       </c>
       <c r="BG5" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="BH5" s="0" t="n">
-        <v>0.36</v>
+        <v>27</v>
       </c>
       <c r="BI5" s="5" t="b">
         <v>true</v>
-      </c>
-      <c r="BK5" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="BL5" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="BM5" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="BN5" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="BO5" s="0" t="n">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="6:6">
       <c r="A6" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B6" s="7">
         <v>42736</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D6" s="7">
-        <v>43119.8575448</v>
+        <v>43126.7719773</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K6" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L6" s="0" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="M6" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6" s="0" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="O6" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P6" s="0" t="n">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R6" s="0" t="n">
-        <v>0.21</v>
+        <v>20</v>
       </c>
       <c r="S6" s="0" t="n">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="T6" s="0" t="n">
-        <v>0.53</v>
+        <v>80</v>
       </c>
       <c r="U6" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V6" s="0" t="n">
-        <v>0.11</v>
+        <v>0</v>
       </c>
       <c r="W6" s="0" t="n">
         <v>0</v>
@@ -1235,58 +1160,58 @@
         <v>0</v>
       </c>
       <c r="Y6" s="0" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="Z6" s="0" t="n">
-        <v>0.47</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AB6" s="0" t="n">
-        <v>0.11</v>
+        <v>17</v>
       </c>
       <c r="AC6" s="0" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="AD6" s="0" t="n">
-        <v>0.32</v>
+        <v>83</v>
       </c>
       <c r="AE6" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF6" s="0" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="AG6" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH6" s="0" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="AI6" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AJ6" s="0" t="n">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AK6" s="0" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="AL6" s="0" t="n">
-        <v>0.16</v>
+        <v>27</v>
       </c>
       <c r="AM6" s="0" t="n">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="AN6" s="0" t="n">
-        <v>0.58</v>
+        <v>73</v>
       </c>
       <c r="AO6" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AP6" s="0" t="n">
-        <v>0.11</v>
+        <v>0</v>
       </c>
       <c r="AQ6" s="0" t="n">
         <v>0</v>
@@ -1295,28 +1220,28 @@
         <v>0</v>
       </c>
       <c r="AS6" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AT6" s="0" t="n">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AU6" s="0" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AV6" s="0" t="n">
-        <v>0.21</v>
+        <v>23</v>
       </c>
       <c r="AW6" s="0" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="AX6" s="0" t="n">
-        <v>0.53</v>
+        <v>77</v>
       </c>
       <c r="AY6" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ6" s="0" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="BA6" s="0" t="n">
         <v>0</v>
@@ -1325,272 +1250,242 @@
         <v>0</v>
       </c>
       <c r="BC6" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BD6" s="0" t="n">
-        <v>0.11</v>
+        <v>0</v>
       </c>
       <c r="BE6" s="0" t="n">
         <v>7</v>
       </c>
       <c r="BF6" s="0" t="n">
-        <v>0.37</v>
+        <v>64</v>
       </c>
       <c r="BG6" s="0" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="BH6" s="0" t="n">
-        <v>0.47</v>
+        <v>36</v>
       </c>
       <c r="BI6" s="5" t="b">
         <v>true</v>
-      </c>
-      <c r="BK6" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="BL6" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="BM6" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="BN6" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="BO6" s="0" t="n">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="7:7">
       <c r="A7" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B7" s="7">
         <v>42736</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="7">
+        <v>43126.7719773</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="7">
-        <v>43119.8575448</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>40</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M7" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O7" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P7" s="0" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="T7" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="U7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="V7" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="W7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="Z7" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="AA7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB7" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="AC7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD7" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="AE7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AI7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ7" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="AK7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL7" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="AM7" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="AN7" s="0" t="n">
+        <v>57.99999999999999</v>
+      </c>
+      <c r="AO7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP7" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="AQ7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT7" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="AU7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AV7" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AW7" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="AX7" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="AY7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="BA7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="BD7" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="BE7" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="R7" s="0" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="S7" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="T7" s="0" t="n">
-        <v>0.36</v>
-      </c>
-      <c r="U7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="AB7" s="0" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="AC7" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD7" s="0" t="n">
-        <v>0.36</v>
-      </c>
-      <c r="AE7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH7" s="0" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="AI7" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ7" s="0" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="AK7" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="AL7" s="0" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="AM7" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="AN7" s="0" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="AO7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR7" s="0" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="AS7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU7" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="AV7" s="0" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="AW7" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="AX7" s="0" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="AY7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BD7" s="0" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="BE7" s="0" t="n">
-        <v>8</v>
-      </c>
       <c r="BF7" s="0" t="n">
-        <v>0.73</v>
+        <v>37</v>
       </c>
       <c r="BG7" s="0" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="BH7" s="0" t="n">
-        <v>0.18</v>
+        <v>47</v>
       </c>
       <c r="BI7" s="5" t="b">
         <v>true</v>
-      </c>
-      <c r="BK7" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="BL7" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="BM7" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="BN7" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="BO7" s="0" t="n">
-        <v>11</v>
       </c>
     </row>
     <row r="8" spans="8:8">
       <c r="A8" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B8" s="7">
         <v>42736</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D8" s="7">
-        <v>43119.8575448</v>
+        <v>43126.7719773</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="K8" s="0" t="n">
         <v>0</v>
@@ -1605,22 +1500,22 @@
         <v>0</v>
       </c>
       <c r="O8" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P8" s="0" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="0" t="n">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="R8" s="0" t="n">
-        <v>0.57</v>
+        <v>64</v>
       </c>
       <c r="S8" s="0" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="T8" s="0" t="n">
-        <v>0.38</v>
+        <v>36</v>
       </c>
       <c r="U8" s="0" t="n">
         <v>0</v>
@@ -1635,22 +1530,22 @@
         <v>0</v>
       </c>
       <c r="Y8" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z8" s="0" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="AA8" s="0" t="n">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="AB8" s="0" t="n">
-        <v>0.57</v>
+        <v>64</v>
       </c>
       <c r="AC8" s="0" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="AD8" s="0" t="n">
-        <v>0.4</v>
+        <v>36</v>
       </c>
       <c r="AE8" s="0" t="n">
         <v>0</v>
@@ -1662,26 +1557,26 @@
         <v>1</v>
       </c>
       <c r="AH8" s="0" t="n">
-        <v>0.02</v>
+        <v>9</v>
       </c>
       <c r="AI8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AJ8" s="0" t="n">
-        <v>0.05</v>
+        <v>18</v>
       </c>
       <c r="AK8" s="0" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="AL8" s="0" t="n">
-        <v>0.5</v>
+        <v>55.00000000000001</v>
       </c>
       <c r="AM8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN8" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="AN8" s="0" t="n">
-        <v>0.43</v>
-      </c>
       <c r="AO8" s="0" t="n">
         <v>0</v>
       </c>
@@ -1692,25 +1587,25 @@
         <v>1</v>
       </c>
       <c r="AR8" s="0" t="n">
-        <v>0.02</v>
+        <v>9</v>
       </c>
       <c r="AS8" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AT8" s="0" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AU8" s="0" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="AV8" s="0" t="n">
-        <v>0.5</v>
+        <v>45</v>
       </c>
       <c r="AW8" s="0" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="AX8" s="0" t="n">
-        <v>0.38</v>
+        <v>45</v>
       </c>
       <c r="AY8" s="0" t="n">
         <v>0</v>
@@ -1725,78 +1620,63 @@
         <v>0</v>
       </c>
       <c r="BC8" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BD8" s="0" t="n">
-        <v>0.05</v>
+        <v>9</v>
       </c>
       <c r="BE8" s="0" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="BF8" s="0" t="n">
-        <v>0.5</v>
+        <v>73</v>
       </c>
       <c r="BG8" s="0" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="BH8" s="0" t="n">
-        <v>0.45</v>
+        <v>18</v>
       </c>
       <c r="BI8" s="5" t="b">
         <v>true</v>
-      </c>
-      <c r="BK8" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="BL8" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="BM8" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="BN8" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="BO8" s="0" t="n">
-        <v>42</v>
       </c>
     </row>
     <row r="9" spans="9:9">
       <c r="A9" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B9" s="7">
         <v>42736</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D9" s="7">
-        <v>43119.8575448</v>
+        <v>43126.7719773</v>
       </c>
       <c r="E9" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="J9" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="K9" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L9" s="0" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="M9" s="0" t="n">
         <v>0</v>
@@ -1805,198 +1685,183 @@
         <v>0</v>
       </c>
       <c r="O9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <v>56.99999999999999</v>
+      </c>
+      <c r="S9" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="T9" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="U9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA9" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="AB9" s="0" t="n">
+        <v>56.99999999999999</v>
+      </c>
+      <c r="AC9" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="AD9" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AK9" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AL9" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="AM9" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="AN9" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="AO9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS9" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="P9" s="0" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="Q9" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="R9" s="0" t="n">
-        <v>0.39</v>
-      </c>
-      <c r="S9" s="0" t="n">
+      <c r="AT9" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="AU9" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AV9" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="AW9" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="AX9" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="T9" s="0" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="U9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="V9" s="0" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="W9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z9" s="0" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="AA9" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="AB9" s="0" t="n">
-        <v>0.38</v>
-      </c>
-      <c r="AC9" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="AD9" s="0" t="n">
-        <v>0.56</v>
-      </c>
-      <c r="AE9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="AF9" s="0" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="AG9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI9" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="AJ9" s="0" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="AK9" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="AL9" s="0" t="n">
-        <v>0.31</v>
-      </c>
-      <c r="AM9" s="0" t="n">
+      <c r="AY9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="BD9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="BE9" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="BF9" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="BG9" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="BH9" s="0" t="n">
         <v>45</v>
-      </c>
-      <c r="AN9" s="0" t="n">
-        <v>0.63</v>
-      </c>
-      <c r="AO9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="AP9" s="0" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="AQ9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS9" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="AT9" s="0" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="AU9" s="0" t="n">
-        <v>31</v>
-      </c>
-      <c r="AV9" s="0" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="AW9" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="AX9" s="0" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="AY9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="AZ9" s="0" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="BA9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BD9" s="0" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="BE9" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="BF9" s="0" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="BG9" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="BH9" s="0" t="n">
-        <v>0.54</v>
       </c>
       <c r="BI9" s="5" t="b">
         <v>true</v>
-      </c>
-      <c r="BK9" s="0" t="n">
-        <v>72</v>
-      </c>
-      <c r="BL9" s="0" t="n">
-        <v>72</v>
-      </c>
-      <c r="BM9" s="0" t="n">
-        <v>72</v>
-      </c>
-      <c r="BN9" s="0" t="n">
-        <v>72</v>
-      </c>
-      <c r="BO9" s="0" t="n">
-        <v>72</v>
       </c>
     </row>
     <row r="10" spans="10:10">
       <c r="A10" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B10" s="7">
         <v>42736</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D10" s="7">
-        <v>43119.8575448</v>
+        <v>43126.7719773</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I10" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="K10" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L10" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M10" s="0" t="n">
         <v>0</v>
@@ -2005,28 +1870,28 @@
         <v>0</v>
       </c>
       <c r="O10" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P10" s="0" t="n">
-        <v>0.09</v>
+        <v>6</v>
       </c>
       <c r="Q10" s="0" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="R10" s="0" t="n">
-        <v>0.43</v>
+        <v>39</v>
       </c>
       <c r="S10" s="0" t="n">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="T10" s="0" t="n">
-        <v>0.48</v>
+        <v>53</v>
       </c>
       <c r="U10" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V10" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W10" s="0" t="n">
         <v>0</v>
@@ -2035,28 +1900,28 @@
         <v>0</v>
       </c>
       <c r="Y10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z10" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="Z10" s="0" t="n">
-        <v>0.07</v>
-      </c>
       <c r="AA10" s="0" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="AB10" s="0" t="n">
-        <v>0.46</v>
+        <v>38</v>
       </c>
       <c r="AC10" s="0" t="n">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="AD10" s="0" t="n">
-        <v>0.46</v>
+        <v>56.00000000000001</v>
       </c>
       <c r="AE10" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF10" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AG10" s="0" t="n">
         <v>0</v>
@@ -2068,55 +1933,55 @@
         <v>3</v>
       </c>
       <c r="AJ10" s="0" t="n">
-        <v>0.06</v>
+        <v>4</v>
       </c>
       <c r="AK10" s="0" t="n">
         <v>22</v>
       </c>
       <c r="AL10" s="0" t="n">
-        <v>0.41</v>
+        <v>31</v>
       </c>
       <c r="AM10" s="0" t="n">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="AN10" s="0" t="n">
-        <v>0.54</v>
+        <v>63</v>
       </c>
       <c r="AO10" s="0" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AP10" s="0" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="AQ10" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AR10" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AS10" s="0" t="n">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="AT10" s="0" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="AU10" s="0" t="n">
-        <v>-1</v>
+        <v>31</v>
       </c>
       <c r="AV10" s="0" t="n">
-        <v>-1</v>
+        <v>43</v>
       </c>
       <c r="AW10" s="0" t="n">
-        <v>-1</v>
+        <v>33</v>
       </c>
       <c r="AX10" s="0" t="n">
-        <v>-1</v>
+        <v>46</v>
       </c>
       <c r="AY10" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AZ10" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA10" s="0" t="n">
         <v>0</v>
@@ -2125,72 +1990,57 @@
         <v>0</v>
       </c>
       <c r="BC10" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="BD10" s="0" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="BE10" s="0" t="n">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="BF10" s="0" t="n">
-        <v>0.33</v>
+        <v>42</v>
       </c>
       <c r="BG10" s="0" t="n">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="BH10" s="0" t="n">
-        <v>0.59</v>
+        <v>54</v>
       </c>
       <c r="BI10" s="5" t="b">
         <v>true</v>
-      </c>
-      <c r="BK10" s="0" t="n">
-        <v>54</v>
-      </c>
-      <c r="BL10" s="0" t="n">
-        <v>54</v>
-      </c>
-      <c r="BM10" s="0" t="n">
-        <v>54</v>
-      </c>
-      <c r="BN10" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="BO10" s="0" t="n">
-        <v>54</v>
       </c>
     </row>
     <row r="11" spans="11:11">
       <c r="A11" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B11" s="7">
         <v>42736</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D11" s="7">
-        <v>43119.8575448</v>
+        <v>43126.7719773</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I11" s="0" t="n">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="K11" s="0" t="n">
         <v>0</v>
@@ -2202,25 +2052,25 @@
         <v>1</v>
       </c>
       <c r="N11" s="0" t="n">
-        <v>0.02</v>
+        <v>2</v>
       </c>
       <c r="O11" s="0" t="n">
         <v>5</v>
       </c>
       <c r="P11" s="0" t="n">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="Q11" s="0" t="n">
         <v>19</v>
       </c>
       <c r="R11" s="0" t="n">
-        <v>0.42</v>
+        <v>42</v>
       </c>
       <c r="S11" s="0" t="n">
         <v>20</v>
       </c>
       <c r="T11" s="0" t="n">
-        <v>0.44</v>
+        <v>44</v>
       </c>
       <c r="U11" s="0" t="n">
         <v>0</v>
@@ -2232,25 +2082,25 @@
         <v>1</v>
       </c>
       <c r="X11" s="0" t="n">
-        <v>0.02</v>
+        <v>2</v>
       </c>
       <c r="Y11" s="0" t="n">
         <v>2</v>
       </c>
       <c r="Z11" s="0" t="n">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="AA11" s="0" t="n">
         <v>23</v>
       </c>
       <c r="AB11" s="0" t="n">
-        <v>0.51</v>
+        <v>51</v>
       </c>
       <c r="AC11" s="0" t="n">
         <v>19</v>
       </c>
       <c r="AD11" s="0" t="n">
-        <v>0.42</v>
+        <v>42</v>
       </c>
       <c r="AE11" s="0" t="n">
         <v>0</v>
@@ -2268,19 +2118,19 @@
         <v>1</v>
       </c>
       <c r="AJ11" s="0" t="n">
-        <v>0.02</v>
+        <v>2</v>
       </c>
       <c r="AK11" s="0" t="n">
         <v>17</v>
       </c>
       <c r="AL11" s="0" t="n">
-        <v>0.38</v>
+        <v>38</v>
       </c>
       <c r="AM11" s="0" t="n">
         <v>27</v>
       </c>
       <c r="AN11" s="0" t="n">
-        <v>0.6</v>
+        <v>60</v>
       </c>
       <c r="AO11" s="0" t="n">
         <v>0</v>
@@ -2298,19 +2148,19 @@
         <v>3</v>
       </c>
       <c r="AT11" s="0" t="n">
-        <v>0.07</v>
+        <v>7.000000000000001</v>
       </c>
       <c r="AU11" s="0" t="n">
         <v>19</v>
       </c>
       <c r="AV11" s="0" t="n">
-        <v>0.42</v>
+        <v>42</v>
       </c>
       <c r="AW11" s="0" t="n">
         <v>23</v>
       </c>
       <c r="AX11" s="0" t="n">
-        <v>0.51</v>
+        <v>51</v>
       </c>
       <c r="AY11" s="0" t="n">
         <v>0</v>
@@ -2328,75 +2178,60 @@
         <v>2</v>
       </c>
       <c r="BD11" s="0" t="n">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="BE11" s="0" t="n">
         <v>20</v>
       </c>
       <c r="BF11" s="0" t="n">
-        <v>0.44</v>
+        <v>44</v>
       </c>
       <c r="BG11" s="0" t="n">
         <v>23</v>
       </c>
       <c r="BH11" s="0" t="n">
-        <v>0.51</v>
+        <v>51</v>
       </c>
       <c r="BI11" s="5" t="b">
         <v>true</v>
-      </c>
-      <c r="BK11" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="BL11" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="BM11" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="BN11" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="BO11" s="0" t="n">
-        <v>45</v>
       </c>
     </row>
     <row r="12" spans="12:12">
       <c r="A12" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B12" s="7">
         <v>42736</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D12" s="7">
-        <v>43119.8575448</v>
+        <v>43126.7719773</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I12" s="0" t="n">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="J12" s="0" t="n">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="K12" s="0" t="n">
         <v>2</v>
       </c>
       <c r="L12" s="0" t="n">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="M12" s="0" t="n">
         <v>0</v>
@@ -2408,25 +2243,25 @@
         <v>4</v>
       </c>
       <c r="P12" s="0" t="n">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="Q12" s="0" t="n">
         <v>24</v>
       </c>
       <c r="R12" s="0" t="n">
-        <v>0.52</v>
+        <v>52</v>
       </c>
       <c r="S12" s="0" t="n">
         <v>16</v>
       </c>
       <c r="T12" s="0" t="n">
-        <v>0.35</v>
+        <v>35</v>
       </c>
       <c r="U12" s="0" t="n">
         <v>2</v>
       </c>
       <c r="V12" s="0" t="n">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="W12" s="0" t="n">
         <v>0</v>
@@ -2438,25 +2273,25 @@
         <v>6</v>
       </c>
       <c r="Z12" s="0" t="n">
-        <v>0.13</v>
+        <v>13</v>
       </c>
       <c r="AA12" s="0" t="n">
         <v>24</v>
       </c>
       <c r="AB12" s="0" t="n">
-        <v>0.52</v>
+        <v>52</v>
       </c>
       <c r="AC12" s="0" t="n">
         <v>14</v>
       </c>
       <c r="AD12" s="0" t="n">
-        <v>0.3</v>
+        <v>30</v>
       </c>
       <c r="AE12" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AF12" s="0" t="n">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="AG12" s="0" t="n">
         <v>0</v>
@@ -2468,25 +2303,25 @@
         <v>7</v>
       </c>
       <c r="AJ12" s="0" t="n">
-        <v>0.15</v>
+        <v>15</v>
       </c>
       <c r="AK12" s="0" t="n">
         <v>21</v>
       </c>
       <c r="AL12" s="0" t="n">
-        <v>0.46</v>
+        <v>46</v>
       </c>
       <c r="AM12" s="0" t="n">
         <v>16</v>
       </c>
       <c r="AN12" s="0" t="n">
-        <v>0.35</v>
+        <v>35</v>
       </c>
       <c r="AO12" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AP12" s="0" t="n">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="AQ12" s="0" t="n">
         <v>0</v>
@@ -2498,25 +2333,25 @@
         <v>6</v>
       </c>
       <c r="AT12" s="0" t="n">
-        <v>0.13</v>
+        <v>13</v>
       </c>
       <c r="AU12" s="0" t="n">
         <v>21</v>
       </c>
       <c r="AV12" s="0" t="n">
-        <v>0.46</v>
+        <v>46</v>
       </c>
       <c r="AW12" s="0" t="n">
         <v>17</v>
       </c>
       <c r="AX12" s="0" t="n">
-        <v>0.37</v>
+        <v>37</v>
       </c>
       <c r="AY12" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AZ12" s="0" t="n">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="BA12" s="0" t="n">
         <v>0</v>
@@ -2528,275 +2363,245 @@
         <v>5</v>
       </c>
       <c r="BD12" s="0" t="n">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="BE12" s="0" t="n">
         <v>21</v>
       </c>
       <c r="BF12" s="0" t="n">
-        <v>0.46</v>
+        <v>46</v>
       </c>
       <c r="BG12" s="0" t="n">
         <v>18</v>
       </c>
       <c r="BH12" s="0" t="n">
-        <v>0.39</v>
+        <v>39</v>
       </c>
       <c r="BI12" s="5" t="b">
         <v>true</v>
-      </c>
-      <c r="BK12" s="0" t="n">
-        <v>46</v>
-      </c>
-      <c r="BL12" s="0" t="n">
-        <v>46</v>
-      </c>
-      <c r="BM12" s="0" t="n">
-        <v>46</v>
-      </c>
-      <c r="BN12" s="0" t="n">
-        <v>46</v>
-      </c>
-      <c r="BO12" s="0" t="n">
-        <v>46</v>
       </c>
     </row>
     <row r="13" spans="13:13">
       <c r="A13" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B13" s="7">
         <v>42736</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D13" s="7">
-        <v>43119.8575448</v>
+        <v>43126.7719773</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I13" s="0" t="n">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="J13" s="0" t="n">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="K13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="L13" s="0" t="n">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="M13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="N13" s="0" t="n">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="O13" s="0" t="n">
         <v>4</v>
       </c>
       <c r="P13" s="0" t="n">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="Q13" s="0" t="n">
         <v>32</v>
       </c>
       <c r="R13" s="0" t="n">
-        <v>0.49</v>
+        <v>49</v>
       </c>
       <c r="S13" s="0" t="n">
         <v>25</v>
       </c>
       <c r="T13" s="0" t="n">
-        <v>0.38</v>
+        <v>38</v>
       </c>
       <c r="U13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="V13" s="0" t="n">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="W13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="X13" s="0" t="n">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="Y13" s="0" t="n">
         <v>9</v>
       </c>
       <c r="Z13" s="0" t="n">
-        <v>0.14</v>
+        <v>14.000000000000002</v>
       </c>
       <c r="AA13" s="0" t="n">
         <v>34</v>
       </c>
       <c r="AB13" s="0" t="n">
-        <v>0.52</v>
+        <v>52</v>
       </c>
       <c r="AC13" s="0" t="n">
         <v>18</v>
       </c>
       <c r="AD13" s="0" t="n">
-        <v>0.28</v>
+        <v>28.000000000000004</v>
       </c>
       <c r="AE13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AF13" s="0" t="n">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="AG13" s="0" t="n">
         <v>3</v>
       </c>
       <c r="AH13" s="0" t="n">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="AI13" s="0" t="n">
         <v>7</v>
       </c>
       <c r="AJ13" s="0" t="n">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="AK13" s="0" t="n">
         <v>31</v>
       </c>
       <c r="AL13" s="0" t="n">
-        <v>0.48</v>
+        <v>48</v>
       </c>
       <c r="AM13" s="0" t="n">
         <v>22</v>
       </c>
       <c r="AN13" s="0" t="n">
-        <v>0.34</v>
+        <v>34</v>
       </c>
       <c r="AO13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AP13" s="0" t="n">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="AQ13" s="0" t="n">
         <v>4</v>
       </c>
       <c r="AR13" s="0" t="n">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="AS13" s="0" t="n">
         <v>7</v>
       </c>
       <c r="AT13" s="0" t="n">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="AU13" s="0" t="n">
         <v>28</v>
       </c>
       <c r="AV13" s="0" t="n">
-        <v>0.43</v>
+        <v>43</v>
       </c>
       <c r="AW13" s="0" t="n">
         <v>24</v>
       </c>
       <c r="AX13" s="0" t="n">
-        <v>0.37</v>
+        <v>37</v>
       </c>
       <c r="AY13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AZ13" s="0" t="n">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="BA13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="BB13" s="0" t="n">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="BC13" s="0" t="n">
         <v>6</v>
       </c>
       <c r="BD13" s="0" t="n">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="BE13" s="0" t="n">
         <v>31</v>
       </c>
       <c r="BF13" s="0" t="n">
-        <v>0.48</v>
+        <v>48</v>
       </c>
       <c r="BG13" s="0" t="n">
         <v>24</v>
       </c>
       <c r="BH13" s="0" t="n">
-        <v>0.37</v>
+        <v>37</v>
       </c>
       <c r="BI13" s="5" t="b">
         <v>true</v>
-      </c>
-      <c r="BK13" s="0" t="n">
-        <v>65</v>
-      </c>
-      <c r="BL13" s="0" t="n">
-        <v>65</v>
-      </c>
-      <c r="BM13" s="0" t="n">
-        <v>65</v>
-      </c>
-      <c r="BN13" s="0" t="n">
-        <v>65</v>
-      </c>
-      <c r="BO13" s="0" t="n">
-        <v>65</v>
       </c>
     </row>
     <row r="14" spans="14:14">
       <c r="A14" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B14" s="7">
         <v>42736</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D14" s="7">
-        <v>43119.8575448</v>
+        <v>43126.7719773</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I14" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J14" s="0" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="K14" s="0" t="n">
         <v>2</v>
       </c>
       <c r="L14" s="0" t="n">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="M14" s="0" t="n">
         <v>0</v>
@@ -2814,19 +2619,19 @@
         <v>5</v>
       </c>
       <c r="R14" s="0" t="n">
-        <v>0.26</v>
+        <v>26</v>
       </c>
       <c r="S14" s="0" t="n">
         <v>12</v>
       </c>
       <c r="T14" s="0" t="n">
-        <v>0.63</v>
+        <v>63</v>
       </c>
       <c r="U14" s="0" t="n">
         <v>2</v>
       </c>
       <c r="V14" s="0" t="n">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="W14" s="0" t="n">
         <v>0</v>
@@ -2838,25 +2643,25 @@
         <v>1</v>
       </c>
       <c r="Z14" s="0" t="n">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="AA14" s="0" t="n">
         <v>4</v>
       </c>
       <c r="AB14" s="0" t="n">
-        <v>0.21</v>
+        <v>21</v>
       </c>
       <c r="AC14" s="0" t="n">
         <v>12</v>
       </c>
       <c r="AD14" s="0" t="n">
-        <v>0.63</v>
+        <v>63</v>
       </c>
       <c r="AE14" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AF14" s="0" t="n">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="AG14" s="0" t="n">
         <v>0</v>
@@ -2874,19 +2679,19 @@
         <v>4</v>
       </c>
       <c r="AL14" s="0" t="n">
-        <v>0.21</v>
+        <v>21</v>
       </c>
       <c r="AM14" s="0" t="n">
         <v>13</v>
       </c>
       <c r="AN14" s="0" t="n">
-        <v>0.68</v>
+        <v>68</v>
       </c>
       <c r="AO14" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AP14" s="0" t="n">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="AQ14" s="0" t="n">
         <v>0</v>
@@ -2904,19 +2709,19 @@
         <v>4</v>
       </c>
       <c r="AV14" s="0" t="n">
-        <v>0.21</v>
+        <v>21</v>
       </c>
       <c r="AW14" s="0" t="n">
         <v>13</v>
       </c>
       <c r="AX14" s="0" t="n">
-        <v>0.68</v>
+        <v>68</v>
       </c>
       <c r="AY14" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AZ14" s="0" t="n">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="BA14" s="0" t="n">
         <v>0</v>
@@ -2934,63 +2739,48 @@
         <v>4</v>
       </c>
       <c r="BF14" s="0" t="n">
-        <v>0.21</v>
+        <v>21</v>
       </c>
       <c r="BG14" s="0" t="n">
         <v>13</v>
       </c>
       <c r="BH14" s="0" t="n">
-        <v>0.68</v>
+        <v>68</v>
       </c>
       <c r="BI14" s="5" t="b">
         <v>true</v>
-      </c>
-      <c r="BK14" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="BL14" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="BM14" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="BN14" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="BO14" s="0" t="n">
-        <v>19</v>
       </c>
     </row>
     <row r="15" spans="15:15">
       <c r="A15" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B15" s="7">
         <v>42736</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D15" s="7">
-        <v>43119.8575448</v>
+        <v>43126.7719773</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I15" s="0" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J15" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" s="0" t="n">
         <v>0</v>
@@ -3020,7 +2810,7 @@
         <v>1</v>
       </c>
       <c r="T15" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="U15" s="0" t="n">
         <v>0</v>
@@ -3050,7 +2840,7 @@
         <v>1</v>
       </c>
       <c r="AD15" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="AE15" s="0" t="n">
         <v>0</v>
@@ -3080,7 +2870,7 @@
         <v>1</v>
       </c>
       <c r="AN15" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="AO15" s="0" t="n">
         <v>0</v>
@@ -3110,7 +2900,7 @@
         <v>1</v>
       </c>
       <c r="AX15" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="AY15" s="0" t="n">
         <v>0</v>
@@ -3140,63 +2930,48 @@
         <v>1</v>
       </c>
       <c r="BH15" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="BI15" s="5" t="b">
         <v>true</v>
-      </c>
-      <c r="BK15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BL15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BM15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BN15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BO15" s="0" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="16" spans="16:16">
       <c r="A16" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B16" s="7">
         <v>42736</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D16" s="7">
-        <v>43119.8575448</v>
+        <v>43126.7719773</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I16" s="0" t="n">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="J16" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L16" s="0" t="n">
-        <v>0.17</v>
+        <v>17</v>
       </c>
       <c r="M16" s="0" t="n">
         <v>0</v>
@@ -3214,19 +2989,19 @@
         <v>2</v>
       </c>
       <c r="R16" s="0" t="n">
-        <v>0.33</v>
+        <v>33</v>
       </c>
       <c r="S16" s="0" t="n">
         <v>3</v>
       </c>
       <c r="T16" s="0" t="n">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="U16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="V16" s="0" t="n">
-        <v>0.17</v>
+        <v>17</v>
       </c>
       <c r="W16" s="0" t="n">
         <v>0</v>
@@ -3238,25 +3013,25 @@
         <v>1</v>
       </c>
       <c r="Z16" s="0" t="n">
-        <v>0.17</v>
+        <v>17</v>
       </c>
       <c r="AA16" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AB16" s="0" t="n">
-        <v>0.33</v>
+        <v>33</v>
       </c>
       <c r="AC16" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AD16" s="0" t="n">
-        <v>0.33</v>
+        <v>33</v>
       </c>
       <c r="AE16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AF16" s="0" t="n">
-        <v>0.17</v>
+        <v>17</v>
       </c>
       <c r="AG16" s="0" t="n">
         <v>0</v>
@@ -3274,19 +3049,19 @@
         <v>2</v>
       </c>
       <c r="AL16" s="0" t="n">
-        <v>0.33</v>
+        <v>33</v>
       </c>
       <c r="AM16" s="0" t="n">
         <v>3</v>
       </c>
       <c r="AN16" s="0" t="n">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="AO16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AP16" s="0" t="n">
-        <v>0.17</v>
+        <v>17</v>
       </c>
       <c r="AQ16" s="0" t="n">
         <v>0</v>
@@ -3304,19 +3079,19 @@
         <v>2</v>
       </c>
       <c r="AV16" s="0" t="n">
-        <v>0.33</v>
+        <v>33</v>
       </c>
       <c r="AW16" s="0" t="n">
         <v>3</v>
       </c>
       <c r="AX16" s="0" t="n">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="AY16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AZ16" s="0" t="n">
-        <v>0.17</v>
+        <v>17</v>
       </c>
       <c r="BA16" s="0" t="n">
         <v>0</v>
@@ -3334,63 +3109,48 @@
         <v>2</v>
       </c>
       <c r="BF16" s="0" t="n">
-        <v>0.33</v>
+        <v>33</v>
       </c>
       <c r="BG16" s="0" t="n">
         <v>3</v>
       </c>
       <c r="BH16" s="0" t="n">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="BI16" s="5" t="b">
         <v>true</v>
-      </c>
-      <c r="BK16" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="BL16" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="BM16" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="BN16" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="BO16" s="0" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="17" spans="17:17">
       <c r="A17" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B17" s="7">
         <v>42736</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D17" s="7">
-        <v>43119.8575448</v>
+        <v>43126.7719773</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I17" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J17" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="0" t="n">
         <v>0</v>
@@ -3414,7 +3174,7 @@
         <v>1</v>
       </c>
       <c r="R17" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="S17" s="0" t="n">
         <v>0</v>
@@ -3444,7 +3204,7 @@
         <v>1</v>
       </c>
       <c r="AB17" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="AC17" s="0" t="n">
         <v>0</v>
@@ -3474,7 +3234,7 @@
         <v>1</v>
       </c>
       <c r="AL17" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="AM17" s="0" t="n">
         <v>0</v>
@@ -3498,7 +3258,7 @@
         <v>1</v>
       </c>
       <c r="AT17" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="AU17" s="0" t="n">
         <v>0</v>
@@ -3534,7 +3294,7 @@
         <v>1</v>
       </c>
       <c r="BF17" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="BG17" s="0" t="n">
         <v>0</v>
@@ -3544,53 +3304,38 @@
       </c>
       <c r="BI17" s="5" t="b">
         <v>true</v>
-      </c>
-      <c r="BK17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BL17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BM17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BN17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BO17" s="0" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="18" spans="18:18">
       <c r="A18" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B18" s="7">
         <v>42736</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D18" s="7">
-        <v>43119.8575448</v>
+        <v>43126.7719773</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I18" s="0" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="J18" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K18" s="0" t="n">
         <v>0</v>
@@ -3620,7 +3365,7 @@
         <v>2</v>
       </c>
       <c r="T18" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="U18" s="0" t="n">
         <v>0</v>
@@ -3644,13 +3389,13 @@
         <v>1</v>
       </c>
       <c r="AB18" s="0" t="n">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="AC18" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AD18" s="0" t="n">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="AE18" s="0" t="n">
         <v>0</v>
@@ -3680,7 +3425,7 @@
         <v>2</v>
       </c>
       <c r="AN18" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="AO18" s="0" t="n">
         <v>0</v>
@@ -3710,7 +3455,7 @@
         <v>2</v>
       </c>
       <c r="AX18" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="AY18" s="0" t="n">
         <v>0</v>
@@ -3740,57 +3485,42 @@
         <v>2</v>
       </c>
       <c r="BH18" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="BI18" s="5" t="b">
         <v>true</v>
-      </c>
-      <c r="BK18" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="BL18" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="BM18" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="BN18" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="BO18" s="0" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="19" spans="19:19">
       <c r="A19" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B19" s="7">
         <v>42736</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D19" s="7">
-        <v>43119.8575448</v>
+        <v>43126.7719773</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I19" s="0" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J19" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" s="0" t="n">
         <v>0</v>
@@ -3820,7 +3550,7 @@
         <v>1</v>
       </c>
       <c r="T19" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="U19" s="0" t="n">
         <v>0</v>
@@ -3850,7 +3580,7 @@
         <v>1</v>
       </c>
       <c r="AD19" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="AE19" s="0" t="n">
         <v>0</v>
@@ -3880,7 +3610,7 @@
         <v>1</v>
       </c>
       <c r="AN19" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="AO19" s="0" t="n">
         <v>0</v>
@@ -3910,7 +3640,7 @@
         <v>1</v>
       </c>
       <c r="AX19" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="AY19" s="0" t="n">
         <v>0</v>
@@ -3940,57 +3670,42 @@
         <v>1</v>
       </c>
       <c r="BH19" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="BI19" s="5" t="b">
         <v>true</v>
-      </c>
-      <c r="BK19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BL19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BM19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BN19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BO19" s="0" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="20" spans="20:20">
       <c r="A20" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B20" s="7">
         <v>42736</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D20" s="7">
-        <v>43119.8575448</v>
+        <v>43126.7719773</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I20" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J20" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="0" t="n">
         <v>0</v>
@@ -4014,7 +3729,7 @@
         <v>1</v>
       </c>
       <c r="R20" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="S20" s="0" t="n">
         <v>0</v>
@@ -4050,7 +3765,7 @@
         <v>1</v>
       </c>
       <c r="AD20" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="AE20" s="0" t="n">
         <v>0</v>
@@ -4074,7 +3789,7 @@
         <v>1</v>
       </c>
       <c r="AL20" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="AM20" s="0" t="n">
         <v>0</v>
@@ -4104,7 +3819,7 @@
         <v>1</v>
       </c>
       <c r="AV20" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="AW20" s="0" t="n">
         <v>0</v>
@@ -4134,7 +3849,7 @@
         <v>1</v>
       </c>
       <c r="BF20" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="BG20" s="0" t="n">
         <v>0</v>
@@ -4144,21 +3859,6 @@
       </c>
       <c r="BI20" s="5" t="b">
         <v>true</v>
-      </c>
-      <c r="BK20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BL20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BM20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BN20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BO20" s="0" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed exel uploading to github
</commit_message>
<xml_diff>
--- a/commonMetricsReport.xlsx
+++ b/commonMetricsReport.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Reporting Information</t>
   </si>
@@ -106,58 +106,70 @@
     <t>John Doe</t>
   </si>
   <si>
+    <t>Marketing Public Health</t>
+  </si>
+  <si>
+    <t>Maintaining Safe Recreational Waters</t>
+  </si>
+  <si>
+    <t>Massachusetts Public Health Inspector Training: Housing</t>
+  </si>
+  <si>
+    <t>Monitoring for Cyanobacteria</t>
+  </si>
+  <si>
+    <t>Housing Certificate Program Final Assessment</t>
+  </si>
+  <si>
+    <t>Introduction to Outreach Methods and Strategies</t>
+  </si>
+  <si>
+    <t>Coaching Skills</t>
+  </si>
+  <si>
+    <t>Effective Meetings</t>
+  </si>
+  <si>
+    <t>Ten Essential Services of Public Health in Action</t>
+  </si>
+  <si>
+    <t>Grant Writing Basics</t>
+  </si>
+  <si>
+    <t>Substance Use Disorders and Models for Supporting Recovery</t>
+  </si>
+  <si>
+    <t>Community Health Assessment: Using Health Models to Explore the Determinants of Health</t>
+  </si>
+  <si>
+    <t>LPHI Emergency Preparedness Training Certificate</t>
+  </si>
+  <si>
+    <t>Numbers in Health:  Make the Meaning Clear</t>
+  </si>
+  <si>
+    <t>Human Health Effects of Climate Change</t>
+  </si>
+  <si>
+    <t>Medication Administration in a School Setting: School Nursing Practice in Massachusetts</t>
+  </si>
+  <si>
+    <t>Introduction to Environmental Health for New Hampshire Health Officers</t>
+  </si>
+  <si>
+    <t>Heyo</t>
+  </si>
+  <si>
+    <t>Jake</t>
+  </si>
+  <si>
     <t>Onboarding New Employees</t>
   </si>
   <si>
-    <t>Marketing Public Health</t>
-  </si>
-  <si>
-    <t>Maintaining Safe Recreational Waters</t>
-  </si>
-  <si>
-    <t>Massachusetts Public Health Inspector Training: Housing</t>
-  </si>
-  <si>
-    <t>Monitoring for Cyanobacteria</t>
-  </si>
-  <si>
-    <t>Housing Certificate Program Final Assessment</t>
-  </si>
-  <si>
-    <t>Introduction to Outreach Methods and Strategies</t>
-  </si>
-  <si>
-    <t>Coaching Skills</t>
-  </si>
-  <si>
-    <t>Effective Meetings</t>
-  </si>
-  <si>
-    <t>Ten Essential Services of Public Health in Action</t>
-  </si>
-  <si>
-    <t>Grant Writing Basics</t>
-  </si>
-  <si>
-    <t>Substance Use Disorders and Models for Supporting Recovery</t>
-  </si>
-  <si>
-    <t>Community Health Assessment: Using Health Models to Explore the Determinants of Health</t>
-  </si>
-  <si>
-    <t>LPHI Emergency Preparedness Training Certificate</t>
-  </si>
-  <si>
-    <t>Numbers in Health:  Make the Meaning Clear</t>
-  </si>
-  <si>
-    <t>Human Health Effects of Climate Change</t>
-  </si>
-  <si>
-    <t>Medication Administration in a School Setting: School Nursing Practice in Massachusetts</t>
-  </si>
-  <si>
-    <t>Introduction to Environmental Health for New Hampshire Health Officers</t>
+    <t>Public health sciences skills</t>
+  </si>
+  <si>
+    <t>Archived/Self-paced Distance Learning</t>
   </si>
 </sst>
 </file>
@@ -542,7 +554,7 @@
         <v>30</v>
       </c>
       <c r="D3" s="7">
-        <v>43126.7719773</v>
+        <v>43133.5445132</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>31</v>
@@ -557,16 +569,16 @@
         <v>0</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>76</v>
+        <v>121</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" s="0" t="n">
         <v>0</v>
@@ -575,142 +587,142 @@
         <v>0</v>
       </c>
       <c r="O3" s="0" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="P3" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="T3" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="U3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="W3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="Z3" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="AA3" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="AB3" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="AC3" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="AD3" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="AE3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AJ3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="AK3" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="AL3" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="AM3" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="AN3" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="AO3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AQ3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="Q3" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="R3" s="0" t="n">
-        <v>43</v>
-      </c>
-      <c r="S3" s="0" t="n">
-        <v>26</v>
-      </c>
-      <c r="T3" s="0" t="n">
-        <v>48</v>
-      </c>
-      <c r="U3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z3" s="0" t="n">
-        <v>7.000000000000001</v>
-      </c>
-      <c r="AA3" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="AB3" s="0" t="n">
-        <v>46</v>
-      </c>
-      <c r="AC3" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="AD3" s="0" t="n">
-        <v>46</v>
-      </c>
-      <c r="AE3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="AJ3" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="AK3" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="AL3" s="0" t="n">
+      <c r="AT3" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="AU3" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="AV3" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="AW3" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="AX3" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="AY3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC3" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="BD3" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="BE3" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="AM3" s="0" t="n">
-        <v>29</v>
-      </c>
-      <c r="AN3" s="0" t="n">
-        <v>54</v>
-      </c>
-      <c r="AO3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AP3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AQ3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AR3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AS3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AT3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AU3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AV3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AW3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AX3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AY3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="BD3" s="0" t="n">
-        <v>7.000000000000001</v>
-      </c>
-      <c r="BE3" s="0" t="n">
-        <v>18</v>
-      </c>
       <c r="BF3" s="0" t="n">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="BG3" s="0" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="BH3" s="0" t="n">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="BI3" s="5" t="b">
         <v>true</v>
@@ -727,7 +739,7 @@
         <v>30</v>
       </c>
       <c r="D4" s="7">
-        <v>43126.7719773</v>
+        <v>43133.5445132</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>32</v>
@@ -742,46 +754,46 @@
         <v>0</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>121</v>
+        <v>31</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>82</v>
+        <v>22</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="M4" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O4" s="0" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="P4" s="0" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="Q4" s="0" t="n">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="R4" s="0" t="n">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="S4" s="0" t="n">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="T4" s="0" t="n">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="U4" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="V4" s="0" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="W4" s="0" t="n">
         <v>0</v>
@@ -790,58 +802,58 @@
         <v>0</v>
       </c>
       <c r="Y4" s="0" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="Z4" s="0" t="n">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="AA4" s="0" t="n">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="AB4" s="0" t="n">
-        <v>55.00000000000001</v>
+        <v>32</v>
       </c>
       <c r="AC4" s="0" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="AD4" s="0" t="n">
-        <v>28.999999999999996</v>
+        <v>18</v>
       </c>
       <c r="AE4" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AF4" s="0" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="AG4" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH4" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AI4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AJ4" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="AK4" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="AJ4" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="AK4" s="0" t="n">
-        <v>38</v>
-      </c>
       <c r="AL4" s="0" t="n">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="AM4" s="0" t="n">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="AN4" s="0" t="n">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="AO4" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AP4" s="0" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="AQ4" s="0" t="n">
         <v>0</v>
@@ -850,52 +862,52 @@
         <v>0</v>
       </c>
       <c r="AS4" s="0" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="AT4" s="0" t="n">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="AU4" s="0" t="n">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="AV4" s="0" t="n">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="AW4" s="0" t="n">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="AX4" s="0" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="AY4" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AZ4" s="0" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="BA4" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB4" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BC4" s="0" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="BD4" s="0" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="BE4" s="0" t="n">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="BF4" s="0" t="n">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="BG4" s="0" t="n">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="BH4" s="0" t="n">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="BI4" s="5" t="b">
         <v>true</v>
@@ -912,7 +924,7 @@
         <v>30</v>
       </c>
       <c r="D5" s="7">
-        <v>43126.7719773</v>
+        <v>43133.5445132</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>33</v>
@@ -927,46 +939,46 @@
         <v>0</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L5" s="0" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="M5" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O5" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P5" s="0" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="0" t="n">
         <v>6</v>
       </c>
       <c r="R5" s="0" t="n">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="S5" s="0" t="n">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="T5" s="0" t="n">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="U5" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="V5" s="0" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="W5" s="0" t="n">
         <v>0</v>
@@ -975,28 +987,28 @@
         <v>0</v>
       </c>
       <c r="Y5" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="Z5" s="0" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="AA5" s="0" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AB5" s="0" t="n">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="AC5" s="0" t="n">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="AD5" s="0" t="n">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="AE5" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AF5" s="0" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="AG5" s="0" t="n">
         <v>0</v>
@@ -1005,28 +1017,28 @@
         <v>0</v>
       </c>
       <c r="AI5" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AJ5" s="0" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="AK5" s="0" t="n">
         <v>8</v>
       </c>
       <c r="AL5" s="0" t="n">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="AM5" s="0" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="AN5" s="0" t="n">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="AO5" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AP5" s="0" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="AQ5" s="0" t="n">
         <v>0</v>
@@ -1035,52 +1047,52 @@
         <v>0</v>
       </c>
       <c r="AS5" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AT5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AV5" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="AU5" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="AV5" s="0" t="n">
-        <v>27</v>
-      </c>
       <c r="AW5" s="0" t="n">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="AX5" s="0" t="n">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="AY5" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AZ5" s="0" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="BA5" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB5" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="BC5" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BD5" s="0" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="BE5" s="0" t="n">
         <v>7</v>
       </c>
       <c r="BF5" s="0" t="n">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="BG5" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="BH5" s="0" t="n">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="BI5" s="5" t="b">
         <v>true</v>
@@ -1097,7 +1109,7 @@
         <v>30</v>
       </c>
       <c r="D6" s="7">
-        <v>43126.7719773</v>
+        <v>43133.5445132</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>34</v>
@@ -1112,106 +1124,106 @@
         <v>0</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="K6" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M6" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O6" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P6" s="0" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="T6" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="U6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="V6" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="W6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="Z6" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="AA6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB6" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="AC6" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="R6" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="S6" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="T6" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="U6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="0" t="n">
+      <c r="AD6" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="AE6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="AB6" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="AC6" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="AD6" s="0" t="n">
-        <v>83</v>
-      </c>
-      <c r="AE6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="AG6" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH6" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI6" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ6" s="0" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AK6" s="0" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="AL6" s="0" t="n">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="AM6" s="0" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="AN6" s="0" t="n">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="AO6" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP6" s="0" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AQ6" s="0" t="n">
         <v>0</v>
@@ -1220,28 +1232,28 @@
         <v>0</v>
       </c>
       <c r="AS6" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AT6" s="0" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AU6" s="0" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AV6" s="0" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AW6" s="0" t="n">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="AX6" s="0" t="n">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="AY6" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ6" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BA6" s="0" t="n">
         <v>0</v>
@@ -1250,22 +1262,22 @@
         <v>0</v>
       </c>
       <c r="BC6" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BD6" s="0" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="BE6" s="0" t="n">
         <v>7</v>
       </c>
       <c r="BF6" s="0" t="n">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="BG6" s="0" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="BH6" s="0" t="n">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="BI6" s="5" t="b">
         <v>true</v>
@@ -1282,7 +1294,7 @@
         <v>30</v>
       </c>
       <c r="D7" s="7">
-        <v>43126.7719773</v>
+        <v>43133.5445132</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>35</v>
@@ -1297,160 +1309,160 @@
         <v>0</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="T7" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="U7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AB7" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="AC7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD7" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="AE7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH7" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="AI7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ7" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="AK7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AL7" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="AM7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN7" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="AO7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR7" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="AS7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="M7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N7" s="0" t="n">
+      <c r="AV7" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="AW7" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="O7" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="P7" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="Q7" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="R7" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="S7" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="T7" s="0" t="n">
-        <v>53</v>
-      </c>
-      <c r="U7" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="V7" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="W7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="0" t="n">
+      <c r="AX7" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="AY7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BD7" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="Z7" s="0" t="n">
-        <v>47</v>
-      </c>
-      <c r="AA7" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="AB7" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="AC7" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="AD7" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="AE7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF7" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="AG7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH7" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="AI7" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="AJ7" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="AK7" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="AL7" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="AM7" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="AN7" s="0" t="n">
-        <v>57.99999999999999</v>
-      </c>
-      <c r="AO7" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="AP7" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="AQ7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS7" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="AT7" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="AU7" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="AV7" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="AW7" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="AX7" s="0" t="n">
-        <v>53</v>
-      </c>
-      <c r="AY7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ7" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="BA7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC7" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="BD7" s="0" t="n">
-        <v>11</v>
-      </c>
       <c r="BE7" s="0" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BF7" s="0" t="n">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="BG7" s="0" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="BH7" s="0" t="n">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="BI7" s="5" t="b">
         <v>true</v>
@@ -1467,7 +1479,7 @@
         <v>30</v>
       </c>
       <c r="D8" s="7">
-        <v>43126.7719773</v>
+        <v>43133.5445132</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>36</v>
@@ -1482,10 +1494,10 @@
         <v>0</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="K8" s="0" t="n">
         <v>0</v>
@@ -1500,142 +1512,142 @@
         <v>0</v>
       </c>
       <c r="O8" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P8" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q8" s="0" t="n">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="R8" s="0" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="S8" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="T8" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="U8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA8" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="AB8" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="AC8" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="AD8" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AK8" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AL8" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="AM8" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="AN8" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="AO8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS8" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="T8" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="U8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="AB8" s="0" t="n">
-        <v>64</v>
-      </c>
-      <c r="AC8" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD8" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="AE8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH8" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="AI8" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ8" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="AK8" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="AL8" s="0" t="n">
-        <v>55.00000000000001</v>
-      </c>
-      <c r="AM8" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="AN8" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="AO8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR8" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="AS8" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="AT8" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AU8" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AV8" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="AW8" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="AX8" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="AY8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="BD8" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="AV8" s="0" t="n">
+      <c r="BE8" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="BF8" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="BG8" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="BH8" s="0" t="n">
         <v>45</v>
-      </c>
-      <c r="AW8" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="AX8" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="AY8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BD8" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="BE8" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="BF8" s="0" t="n">
-        <v>73</v>
-      </c>
-      <c r="BG8" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="BH8" s="0" t="n">
-        <v>18</v>
       </c>
       <c r="BI8" s="5" t="b">
         <v>true</v>
@@ -1652,7 +1664,7 @@
         <v>30</v>
       </c>
       <c r="D9" s="7">
-        <v>43126.7719773</v>
+        <v>43133.5445132</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>37</v>
@@ -1667,160 +1679,160 @@
         <v>0</v>
       </c>
       <c r="I9" s="0" t="n">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="J9" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="S9" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="T9" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="U9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="V9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="W9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA9" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="AB9" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="AC9" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="AD9" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="AE9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AK9" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="AL9" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="AM9" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="AN9" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="AO9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AQ9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AT9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AU9" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="AV9" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="AW9" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="AX9" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="AY9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AZ9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="BA9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BD9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BE9" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="BF9" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="K9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="P9" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q9" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="R9" s="0" t="n">
-        <v>56.99999999999999</v>
-      </c>
-      <c r="S9" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="T9" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="U9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA9" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="AB9" s="0" t="n">
-        <v>56.99999999999999</v>
-      </c>
-      <c r="AC9" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="AD9" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="AE9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="AI9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ9" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="AK9" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="AL9" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="AM9" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="AN9" s="0" t="n">
-        <v>43</v>
-      </c>
-      <c r="AO9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="AS9" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="AT9" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="AU9" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="AV9" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="AW9" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="AX9" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="AY9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="BD9" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="BE9" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="BF9" s="0" t="n">
-        <v>50</v>
-      </c>
       <c r="BG9" s="0" t="n">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="BH9" s="0" t="n">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="BI9" s="5" t="b">
         <v>true</v>
@@ -1837,7 +1849,7 @@
         <v>30</v>
       </c>
       <c r="D10" s="7">
-        <v>43126.7719773</v>
+        <v>43133.5445132</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>38</v>
@@ -1852,160 +1864,160 @@
         <v>0</v>
       </c>
       <c r="I10" s="0" t="n">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="K10" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L10" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M10" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O10" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P10" s="0" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="Q10" s="0" t="n">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="R10" s="0" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="S10" s="0" t="n">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="T10" s="0" t="n">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="U10" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V10" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W10" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X10" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y10" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Z10" s="0" t="n">
         <v>4</v>
       </c>
       <c r="AA10" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="AB10" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="AC10" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="AD10" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="AE10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK10" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="AL10" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="AM10" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="AB10" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="AC10" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="AD10" s="0" t="n">
-        <v>56.00000000000001</v>
-      </c>
-      <c r="AE10" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="AF10" s="0" t="n">
+      <c r="AN10" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="AO10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS10" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="AG10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI10" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="AJ10" s="0" t="n">
+      <c r="AT10" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AU10" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="AV10" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="AW10" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="AX10" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="AY10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="BD10" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="AK10" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="AL10" s="0" t="n">
-        <v>31</v>
-      </c>
-      <c r="AM10" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="AN10" s="0" t="n">
-        <v>63</v>
-      </c>
-      <c r="AO10" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="AP10" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="AQ10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS10" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="AT10" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="AU10" s="0" t="n">
-        <v>31</v>
-      </c>
-      <c r="AV10" s="0" t="n">
-        <v>43</v>
-      </c>
-      <c r="AW10" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="AX10" s="0" t="n">
-        <v>46</v>
-      </c>
-      <c r="AY10" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="AZ10" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="BA10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BD10" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="BE10" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="BF10" s="0" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="BG10" s="0" t="n">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="BH10" s="0" t="n">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="BI10" s="5" t="b">
         <v>true</v>
@@ -2022,7 +2034,7 @@
         <v>30</v>
       </c>
       <c r="D11" s="7">
-        <v>43126.7719773</v>
+        <v>43133.5445132</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>39</v>
@@ -2037,160 +2049,160 @@
         <v>0</v>
       </c>
       <c r="I11" s="0" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K11" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L11" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M11" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P11" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="S11" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="T11" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="U11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="V11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="W11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z11" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="AA11" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="AB11" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="AC11" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="AD11" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AJ11" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="AK11" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AL11" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="AM11" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="AN11" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="AO11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AQ11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS11" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AT11" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="AU11" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AV11" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="AW11" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="AX11" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="AY11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AZ11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="BA11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC11" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="P11" s="0" t="n">
+      <c r="BD11" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="Q11" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="R11" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="S11" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="T11" s="0" t="n">
-        <v>44</v>
-      </c>
-      <c r="U11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="V11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="X11" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="Y11" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z11" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="AA11" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="AB11" s="0" t="n">
-        <v>51</v>
-      </c>
-      <c r="AC11" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="AD11" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="AE11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ11" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="AK11" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="AL11" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="AM11" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="AN11" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="AO11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS11" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="AT11" s="0" t="n">
-        <v>7.000000000000001</v>
-      </c>
-      <c r="AU11" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="AV11" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="AW11" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="AX11" s="0" t="n">
-        <v>51</v>
-      </c>
-      <c r="AY11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC11" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="BD11" s="0" t="n">
-        <v>4</v>
-      </c>
       <c r="BE11" s="0" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="BF11" s="0" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="BG11" s="0" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="BH11" s="0" t="n">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="BI11" s="5" t="b">
         <v>true</v>
@@ -2207,7 +2219,7 @@
         <v>30</v>
       </c>
       <c r="D12" s="7">
-        <v>43126.7719773</v>
+        <v>43133.5445132</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>40</v>
@@ -2222,127 +2234,127 @@
         <v>0</v>
       </c>
       <c r="I12" s="0" t="n">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="J12" s="0" t="n">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="K12" s="0" t="n">
         <v>2</v>
       </c>
       <c r="L12" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M12" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N12" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O12" s="0" t="n">
         <v>4</v>
       </c>
       <c r="P12" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="S12" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="T12" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="U12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="V12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="W12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="X12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y12" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="Q12" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="R12" s="0" t="n">
-        <v>52</v>
-      </c>
-      <c r="S12" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="T12" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="U12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="V12" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="W12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="0" t="n">
-        <v>6</v>
-      </c>
       <c r="Z12" s="0" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AA12" s="0" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="AB12" s="0" t="n">
         <v>52</v>
       </c>
       <c r="AC12" s="0" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="AD12" s="0" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AE12" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AF12" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG12" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH12" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI12" s="0" t="n">
         <v>7</v>
       </c>
       <c r="AJ12" s="0" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AK12" s="0" t="n">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="AL12" s="0" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AM12" s="0" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="AN12" s="0" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AO12" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AP12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AQ12" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="AQ12" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="AR12" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AS12" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AT12" s="0" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AU12" s="0" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="AV12" s="0" t="n">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="AW12" s="0" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="AX12" s="0" t="n">
         <v>37</v>
@@ -2351,31 +2363,31 @@
         <v>2</v>
       </c>
       <c r="AZ12" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="BA12" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BB12" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BC12" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BD12" s="0" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="BE12" s="0" t="n">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="BF12" s="0" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="BG12" s="0" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="BH12" s="0" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="BI12" s="5" t="b">
         <v>true</v>
@@ -2392,7 +2404,7 @@
         <v>30</v>
       </c>
       <c r="D13" s="7">
-        <v>43126.7719773</v>
+        <v>43133.5445132</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>41</v>
@@ -2407,160 +2419,160 @@
         <v>0</v>
       </c>
       <c r="I13" s="0" t="n">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="J13" s="0" t="n">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="K13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="L13" s="0" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="M13" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N13" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="R13" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="S13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="T13" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="U13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="V13" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="W13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA13" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="P13" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q13" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="R13" s="0" t="n">
-        <v>49</v>
-      </c>
-      <c r="S13" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="T13" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="U13" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="V13" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="W13" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="X13" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y13" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="Z13" s="0" t="n">
-        <v>14.000000000000002</v>
-      </c>
-      <c r="AA13" s="0" t="n">
-        <v>34</v>
-      </c>
       <c r="AB13" s="0" t="n">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="AC13" s="0" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="AD13" s="0" t="n">
-        <v>28.000000000000004</v>
+        <v>63</v>
       </c>
       <c r="AE13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AF13" s="0" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="AG13" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AH13" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AI13" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AJ13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AL13" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AM13" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="AN13" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="AO13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP13" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="AK13" s="0" t="n">
-        <v>31</v>
-      </c>
-      <c r="AL13" s="0" t="n">
-        <v>48</v>
-      </c>
-      <c r="AM13" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="AN13" s="0" t="n">
-        <v>34</v>
-      </c>
-      <c r="AO13" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="AP13" s="0" t="n">
-        <v>3</v>
-      </c>
       <c r="AQ13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU13" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="AR13" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="AS13" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="AT13" s="0" t="n">
+      <c r="AV13" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AW13" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="AX13" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="AY13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AZ13" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="AU13" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="AV13" s="0" t="n">
-        <v>43</v>
-      </c>
-      <c r="AW13" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="AX13" s="0" t="n">
-        <v>37</v>
-      </c>
-      <c r="AY13" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="AZ13" s="0" t="n">
-        <v>3</v>
-      </c>
       <c r="BA13" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BB13" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BC13" s="0" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="BD13" s="0" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="BE13" s="0" t="n">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="BF13" s="0" t="n">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="BG13" s="0" t="n">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="BH13" s="0" t="n">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="BI13" s="5" t="b">
         <v>true</v>
@@ -2577,7 +2589,7 @@
         <v>30</v>
       </c>
       <c r="D14" s="7">
-        <v>43126.7719773</v>
+        <v>43133.5445132</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>42</v>
@@ -2592,16 +2604,16 @@
         <v>0</v>
       </c>
       <c r="I14" s="0" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="J14" s="0" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="K14" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L14" s="0" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="M14" s="0" t="n">
         <v>0</v>
@@ -2616,22 +2628,22 @@
         <v>0</v>
       </c>
       <c r="Q14" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="R14" s="0" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="S14" s="0" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="T14" s="0" t="n">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="U14" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V14" s="0" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="W14" s="0" t="n">
         <v>0</v>
@@ -2640,28 +2652,28 @@
         <v>0</v>
       </c>
       <c r="Y14" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z14" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AA14" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AB14" s="0" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="AC14" s="0" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="AD14" s="0" t="n">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="AE14" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF14" s="0" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="AG14" s="0" t="n">
         <v>0</v>
@@ -2676,22 +2688,22 @@
         <v>0</v>
       </c>
       <c r="AK14" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AL14" s="0" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="AM14" s="0" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="AN14" s="0" t="n">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="AO14" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AP14" s="0" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="AQ14" s="0" t="n">
         <v>0</v>
@@ -2706,22 +2718,22 @@
         <v>0</v>
       </c>
       <c r="AU14" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AV14" s="0" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="AW14" s="0" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="AX14" s="0" t="n">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="AY14" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ14" s="0" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="BA14" s="0" t="n">
         <v>0</v>
@@ -2736,16 +2748,16 @@
         <v>0</v>
       </c>
       <c r="BE14" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BF14" s="0" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="BG14" s="0" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="BH14" s="0" t="n">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="BI14" s="5" t="b">
         <v>true</v>
@@ -2762,7 +2774,7 @@
         <v>30</v>
       </c>
       <c r="D15" s="7">
-        <v>43126.7719773</v>
+        <v>43133.5445132</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>43</v>
@@ -2777,16 +2789,16 @@
         <v>0</v>
       </c>
       <c r="I15" s="0" t="n">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="J15" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K15" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" s="0" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="M15" s="0" t="n">
         <v>0</v>
@@ -2801,22 +2813,22 @@
         <v>0</v>
       </c>
       <c r="Q15" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R15" s="0" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="S15" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T15" s="0" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="U15" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V15" s="0" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="W15" s="0" t="n">
         <v>0</v>
@@ -2825,28 +2837,28 @@
         <v>0</v>
       </c>
       <c r="Y15" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z15" s="0" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AA15" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB15" s="0" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AC15" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD15" s="0" t="n">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="AE15" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF15" s="0" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AG15" s="0" t="n">
         <v>0</v>
@@ -2861,22 +2873,22 @@
         <v>0</v>
       </c>
       <c r="AK15" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL15" s="0" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AM15" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AN15" s="0" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="AO15" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP15" s="0" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AQ15" s="0" t="n">
         <v>0</v>
@@ -2891,22 +2903,22 @@
         <v>0</v>
       </c>
       <c r="AU15" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AV15" s="0" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AW15" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AX15" s="0" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="AY15" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ15" s="0" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="BA15" s="0" t="n">
         <v>0</v>
@@ -2921,16 +2933,16 @@
         <v>0</v>
       </c>
       <c r="BE15" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BF15" s="0" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="BG15" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BH15" s="0" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="BI15" s="5" t="b">
         <v>true</v>
@@ -2947,7 +2959,7 @@
         <v>30</v>
       </c>
       <c r="D16" s="7">
-        <v>43126.7719773</v>
+        <v>43133.5445132</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>44</v>
@@ -2962,16 +2974,16 @@
         <v>0</v>
       </c>
       <c r="I16" s="0" t="n">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="J16" s="0" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K16" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" s="0" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="M16" s="0" t="n">
         <v>0</v>
@@ -2986,22 +2998,22 @@
         <v>0</v>
       </c>
       <c r="Q16" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R16" s="0" t="n">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="S16" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T16" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="U16" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V16" s="0" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="W16" s="0" t="n">
         <v>0</v>
@@ -3010,28 +3022,28 @@
         <v>0</v>
       </c>
       <c r="Y16" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z16" s="0" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="AA16" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB16" s="0" t="n">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="AC16" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AD16" s="0" t="n">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="AE16" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF16" s="0" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="AG16" s="0" t="n">
         <v>0</v>
@@ -3046,22 +3058,22 @@
         <v>0</v>
       </c>
       <c r="AK16" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL16" s="0" t="n">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="AM16" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AN16" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AO16" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP16" s="0" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="AQ16" s="0" t="n">
         <v>0</v>
@@ -3070,28 +3082,28 @@
         <v>0</v>
       </c>
       <c r="AS16" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT16" s="0" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AU16" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AV16" s="0" t="n">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="AW16" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AX16" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AY16" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ16" s="0" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="BA16" s="0" t="n">
         <v>0</v>
@@ -3106,16 +3118,16 @@
         <v>0</v>
       </c>
       <c r="BE16" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BF16" s="0" t="n">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="BG16" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH16" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="BI16" s="5" t="b">
         <v>true</v>
@@ -3132,7 +3144,7 @@
         <v>30</v>
       </c>
       <c r="D17" s="7">
-        <v>43126.7719773</v>
+        <v>43133.5445132</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>45</v>
@@ -3147,10 +3159,10 @@
         <v>0</v>
       </c>
       <c r="I17" s="0" t="n">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="J17" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K17" s="0" t="n">
         <v>0</v>
@@ -3171,17 +3183,17 @@
         <v>0</v>
       </c>
       <c r="Q17" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="T17" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="S17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T17" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="U17" s="0" t="n">
         <v>0</v>
       </c>
@@ -3204,103 +3216,103 @@
         <v>1</v>
       </c>
       <c r="AB17" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="AC17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD17" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="AE17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN17" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="AC17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL17" s="0" t="n">
+      <c r="AO17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AX17" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="AM17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT17" s="0" t="n">
+      <c r="AY17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="BH17" s="0" t="n">
         <v>100</v>
-      </c>
-      <c r="AU17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BF17" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="BG17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH17" s="0" t="n">
-        <v>0</v>
       </c>
       <c r="BI17" s="5" t="b">
         <v>true</v>
@@ -3317,7 +3329,7 @@
         <v>30</v>
       </c>
       <c r="D18" s="7">
-        <v>43126.7719773</v>
+        <v>43133.5445132</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>46</v>
@@ -3332,10 +3344,10 @@
         <v>0</v>
       </c>
       <c r="I18" s="0" t="n">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="J18" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K18" s="0" t="n">
         <v>0</v>
@@ -3362,7 +3374,7 @@
         <v>0</v>
       </c>
       <c r="S18" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T18" s="0" t="n">
         <v>100</v>
@@ -3386,16 +3398,16 @@
         <v>0</v>
       </c>
       <c r="AA18" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB18" s="0" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC18" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AD18" s="0" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="AE18" s="0" t="n">
         <v>0</v>
@@ -3422,7 +3434,7 @@
         <v>0</v>
       </c>
       <c r="AM18" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN18" s="0" t="n">
         <v>100</v>
@@ -3452,7 +3464,7 @@
         <v>0</v>
       </c>
       <c r="AW18" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AX18" s="0" t="n">
         <v>100</v>
@@ -3482,7 +3494,7 @@
         <v>0</v>
       </c>
       <c r="BG18" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BH18" s="0" t="n">
         <v>100</v>
@@ -3502,7 +3514,7 @@
         <v>30</v>
       </c>
       <c r="D19" s="7">
-        <v>43126.7719773</v>
+        <v>43133.5445132</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>47</v>
@@ -3517,7 +3529,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="0" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="J19" s="0" t="n">
         <v>1</v>
@@ -3541,16 +3553,16 @@
         <v>0</v>
       </c>
       <c r="Q19" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R19" s="0" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S19" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T19" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="U19" s="0" t="n">
         <v>0</v>
@@ -3601,76 +3613,76 @@
         <v>0</v>
       </c>
       <c r="AK19" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL19" s="0" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AM19" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV19" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="AO19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV19" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="AW19" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BF19" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="AY19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF19" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="BG19" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH19" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="BI19" s="5" t="b">
         <v>true</v>
@@ -3678,65 +3690,65 @@
     </row>
     <row r="20" spans="20:20">
       <c r="A20" s="5" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="B20" s="7">
         <v>42736</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="D20" s="7">
-        <v>43126.7719773</v>
+        <v>43133</v>
       </c>
       <c r="E20" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="P20" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q20" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="R20" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="S20" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="T20" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="R20" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="S20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T20" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="U20" s="0" t="n">
         <v>0</v>
       </c>
@@ -3750,22 +3762,22 @@
         <v>0</v>
       </c>
       <c r="Y20" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z20" s="0" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AA20" s="0" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AB20" s="0" t="n">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="AC20" s="0" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="AD20" s="0" t="n">
-        <v>100</v>
+        <v>46</v>
       </c>
       <c r="AE20" s="0" t="n">
         <v>0</v>
@@ -3780,52 +3792,52 @@
         <v>0</v>
       </c>
       <c r="AI20" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ20" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK20" s="0" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="AL20" s="0" t="n">
-        <v>100</v>
+        <v>41</v>
       </c>
       <c r="AM20" s="0" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AN20" s="0" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="AO20" s="0" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AP20" s="0" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AQ20" s="0" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AR20" s="0" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AS20" s="0" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AT20" s="0" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AU20" s="0" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AV20" s="0" t="n">
-        <v>100</v>
+        <v>-1</v>
       </c>
       <c r="AW20" s="0" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AX20" s="0" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AY20" s="0" t="n">
         <v>0</v>
@@ -3840,22 +3852,22 @@
         <v>0</v>
       </c>
       <c r="BC20" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BD20" s="0" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BE20" s="0" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="BF20" s="0" t="n">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="BG20" s="0" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="BH20" s="0" t="n">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="BI20" s="5" t="b">
         <v>true</v>

</xml_diff>